<commit_message>
Completed entering 8PSK and 8APSK-L data
</commit_message>
<xml_diff>
--- a/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
+++ b/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>Bit Rate</t>
   </si>
@@ -142,6 +142,42 @@
   </si>
   <si>
     <t>16APSK 9/10</t>
+  </si>
+  <si>
+    <t>16APSK-L 26/45</t>
+  </si>
+  <si>
+    <t>16APSK-L 3/5</t>
+  </si>
+  <si>
+    <t>16APSK-L 28/45</t>
+  </si>
+  <si>
+    <t>16APSK-L 23/36</t>
+  </si>
+  <si>
+    <t>16APSK-L 25/36</t>
+  </si>
+  <si>
+    <t>16APSK-L 13/18</t>
+  </si>
+  <si>
+    <t>16APSK-L 7/9</t>
+  </si>
+  <si>
+    <t>16APSK-L 77/90</t>
+  </si>
+  <si>
+    <t>16APSK-L 5/9</t>
+  </si>
+  <si>
+    <t>16APSK-L 8/15</t>
+  </si>
+  <si>
+    <t>16APSK-L 1/2</t>
+  </si>
+  <si>
+    <t>16APSK-L 2/3</t>
   </si>
 </sst>
 </file>
@@ -557,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -789,7 +825,7 @@
         <v>0.69444444444444442</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -797,7 +833,7 @@
         <v>0.72222222222222221</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:2">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -805,7 +841,7 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -813,10 +849,10 @@
         <v>0.57777777777777772</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:2">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:2">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
@@ -824,7 +860,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:2">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
@@ -832,7 +868,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:2">
       <c r="A39" s="4" t="s">
         <v>37</v>
       </c>
@@ -840,7 +876,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:2">
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
@@ -848,7 +884,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:2">
       <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
@@ -856,7 +892,7 @@
         <v>0.88888888888888884</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:2">
       <c r="A42" s="3" t="s">
         <v>40</v>
       </c>
@@ -864,25 +900,129 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
+    <row r="43" spans="1:2">
+      <c r="A43" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.57777777777777772</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.62222222222222223</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.63888888888888884</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.69444444444444442</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.72222222222222221</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.85555555555555551</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
         <v>4</v>
       </c>
-      <c r="B45">
+      <c r="B62">
         <v>16200</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C62" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
         <v>7</v>
       </c>
-      <c r="B47">
+      <c r="B64">
         <v>32400</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C64" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed user ====> operator
</commit_message>
<xml_diff>
--- a/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
+++ b/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
@@ -353,13 +353,13 @@
     <t>Users at Fixed Bit Rate</t>
   </si>
   <si>
-    <t>If using a fixed bit rate per user:</t>
-  </si>
-  <si>
-    <t>If using a fixed number of users:</t>
-  </si>
-  <si>
     <t>This means you can change the value</t>
+  </si>
+  <si>
+    <t>If using a fixed bit rate per operator:</t>
+  </si>
+  <si>
+    <t>If using a fixed number of operator:</t>
   </si>
 </sst>
 </file>
@@ -825,7 +825,7 @@
   <dimension ref="A1:G140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -850,12 +850,12 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B5" s="12">
         <v>5000</v>
@@ -866,7 +866,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B6" s="12">
         <v>200</v>

</xml_diff>

<commit_message>
cleaned up headings and boldified everything consistently
</commit_message>
<xml_diff>
--- a/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
+++ b/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14100" yWindow="960" windowWidth="32020" windowHeight="26120" tabRatio="500"/>
+    <workbookView xWindow="13540" yWindow="1100" windowWidth="32020" windowHeight="26120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="114">
   <si>
     <t>Symbol Rate</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Long FECFRAME</t>
   </si>
   <si>
-    <t>bits</t>
-  </si>
-  <si>
     <t>Medium FECFRAME</t>
   </si>
   <si>
@@ -320,12 +317,6 @@
     <t>BPSK-Spread2 code rate 11/45</t>
   </si>
   <si>
-    <t>Modulation Order</t>
-  </si>
-  <si>
-    <t>if</t>
-  </si>
-  <si>
     <t>then</t>
   </si>
   <si>
@@ -360,6 +351,21 @@
   </si>
   <si>
     <t>If using a fixed number of operator:</t>
+  </si>
+  <si>
+    <t>If Modulation</t>
+  </si>
+  <si>
+    <t>Order is</t>
+  </si>
+  <si>
+    <t>64800 bits</t>
+  </si>
+  <si>
+    <t>16200 bits</t>
+  </si>
+  <si>
+    <t>32400 bits</t>
   </si>
 </sst>
 </file>
@@ -825,7 +831,7 @@
   <dimension ref="A1:G140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,39 +846,39 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B5" s="12">
         <v>5000</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B6" s="12">
         <v>200</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -884,49 +890,46 @@
         <v>6000000</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="F10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>64800</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F11" t="s">
-        <v>108</v>
-      </c>
-      <c r="G11" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1">
         <v>0.25</v>
@@ -950,7 +953,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1">
         <v>0.33333333333333331</v>
@@ -973,7 +976,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1">
         <v>0.4</v>
@@ -996,7 +999,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1">
         <v>0.5</v>
@@ -1019,7 +1022,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1">
         <v>0.6</v>
@@ -1042,7 +1045,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1">
         <v>0.66666666666666663</v>
@@ -1065,7 +1068,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="1">
         <v>0.75</v>
@@ -1088,7 +1091,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1">
         <v>0.8</v>
@@ -1111,7 +1114,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="1">
         <v>0.83333333333333337</v>
@@ -1134,7 +1137,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="1">
         <v>0.88888888888888884</v>
@@ -1157,7 +1160,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1">
         <v>0.9</v>
@@ -1180,7 +1183,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1">
         <v>0.52</v>
@@ -1203,7 +1206,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="1">
         <v>0.45</v>
@@ -1226,7 +1229,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" s="1">
         <v>0.55000000000000004</v>
@@ -1255,7 +1258,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="1">
         <v>0.6</v>
@@ -1278,7 +1281,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="1">
         <v>0.66666666666666663</v>
@@ -1301,7 +1304,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="1">
         <v>0.75</v>
@@ -1324,7 +1327,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="1">
         <v>0.83333333333333337</v>
@@ -1347,7 +1350,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" s="1">
         <v>0.88888888888888884</v>
@@ -1370,7 +1373,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="1">
         <v>0.9</v>
@@ -1393,7 +1396,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" s="1">
         <v>0.63888888888888884</v>
@@ -1416,7 +1419,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34" s="1">
         <v>0.69444444444444442</v>
@@ -1439,7 +1442,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" s="1">
         <v>0.72222222222222221</v>
@@ -1462,7 +1465,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" s="1">
         <v>0.55555555555555558</v>
@@ -1485,7 +1488,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" s="1">
         <v>0.57777777777777772</v>
@@ -1514,7 +1517,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" s="1">
         <v>0.66666666666666663</v>
@@ -1537,7 +1540,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="1">
         <v>0.75</v>
@@ -1560,7 +1563,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" s="1">
         <v>0.8</v>
@@ -1583,7 +1586,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B42" s="1">
         <v>0.83333333333333337</v>
@@ -1606,7 +1609,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" s="1">
         <v>0.88888888888888884</v>
@@ -1629,7 +1632,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="1">
         <v>0.9</v>
@@ -1652,7 +1655,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" s="1">
         <v>0.57777777777777772</v>
@@ -1675,7 +1678,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" s="1">
         <v>0.6</v>
@@ -1698,7 +1701,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" s="1">
         <v>0.62222222222222223</v>
@@ -1721,7 +1724,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B48" s="1">
         <v>0.63888888888888884</v>
@@ -1744,7 +1747,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" s="1">
         <v>0.69444444444444442</v>
@@ -1767,7 +1770,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50" s="1">
         <v>0.72222222222222221</v>
@@ -1790,7 +1793,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51" s="1">
         <v>0.77777777777777779</v>
@@ -1813,7 +1816,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B52" s="1">
         <v>0.85555555555555551</v>
@@ -1836,7 +1839,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B53" s="1">
         <v>0.55555555555555558</v>
@@ -1859,7 +1862,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B54" s="1">
         <v>0.53333333333333333</v>
@@ -1882,7 +1885,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B55" s="1">
         <v>0.5</v>
@@ -1905,7 +1908,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B56" s="1">
         <v>0.6</v>
@@ -1928,7 +1931,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B57" s="1">
         <v>0.66666666666666663</v>
@@ -1958,7 +1961,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B59" s="1">
         <v>0.75</v>
@@ -1981,7 +1984,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B60" s="1">
         <v>0.8</v>
@@ -2004,7 +2007,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B61" s="1">
         <v>0.83333333333333337</v>
@@ -2027,7 +2030,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B62" s="1">
         <v>0.88888888888888884</v>
@@ -2050,7 +2053,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B63" s="1">
         <v>0.9</v>
@@ -2073,7 +2076,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B64" s="1">
         <v>0.71111111111111114</v>
@@ -2096,7 +2099,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B65" s="1">
         <v>0.73333333333333328</v>
@@ -2119,7 +2122,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B66" s="1">
         <v>0.77777777777777779</v>
@@ -2142,7 +2145,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B67" s="1">
         <v>0.66666666666666663</v>
@@ -2172,7 +2175,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B69" s="1">
         <v>0.73333333333333328</v>
@@ -2195,7 +2198,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B70" s="1">
         <v>0.77777777777777779</v>
@@ -2218,7 +2221,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B71" s="1">
         <v>0.8</v>
@@ -2241,7 +2244,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B72" s="1">
         <v>0.83333333333333337</v>
@@ -2264,7 +2267,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B73" s="1">
         <v>0.71111111111111114</v>
@@ -2294,7 +2297,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B75" s="1">
         <v>0.75</v>
@@ -2317,7 +2320,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B76" s="1">
         <v>0.77777777777777779</v>
@@ -2340,7 +2343,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B77" s="1">
         <v>0.71111111111111114</v>
@@ -2363,7 +2366,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B78" s="1">
         <v>0.75</v>
@@ -2386,7 +2389,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B79" s="1">
         <v>0.64444444444444449</v>
@@ -2409,7 +2412,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B80" s="1">
         <v>0.66666666666666663</v>
@@ -2432,7 +2435,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B81" s="1">
         <v>0.68888888888888888</v>
@@ -2455,7 +2458,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B82" s="1">
         <v>0.73333333333333328</v>
@@ -2492,11 +2495,8 @@
       <c r="A85" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B85" s="9">
-        <v>16200</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>3</v>
+      <c r="B85" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="E85" s="10"/>
       <c r="F85" s="11"/>
@@ -2504,7 +2504,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B86" s="6">
         <v>0.25</v>
@@ -2527,7 +2527,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B87" s="6">
         <v>0.33333333333333331</v>
@@ -2550,7 +2550,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B88" s="6">
         <v>0.4</v>
@@ -2573,7 +2573,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B89" s="6">
         <v>0.5</v>
@@ -2596,7 +2596,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B90" s="6">
         <v>0.6</v>
@@ -2619,7 +2619,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B91" s="6">
         <v>0.66666666666666663</v>
@@ -2642,7 +2642,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B92" s="6">
         <v>0.75</v>
@@ -2665,7 +2665,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B93" s="6">
         <v>0.8</v>
@@ -2688,7 +2688,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B94" s="6">
         <v>0.83333333333333337</v>
@@ -2711,7 +2711,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B95" s="6">
         <v>0.88888888888888884</v>
@@ -2734,7 +2734,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B96" s="6">
         <v>0.24444444444444444</v>
@@ -2757,7 +2757,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B97" s="6">
         <v>0.26666666666666666</v>
@@ -2780,7 +2780,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B98" s="6">
         <v>0.31111111111111112</v>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B99" s="6">
         <v>0.46666666666666667</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B100" s="6">
         <v>0.53333333333333333</v>
@@ -2849,7 +2849,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B101" s="6">
         <v>0.71111111111111114</v>
@@ -2878,7 +2878,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B103" s="6">
         <v>0.6</v>
@@ -2901,7 +2901,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B104" s="6">
         <v>0.66666666666666663</v>
@@ -2924,7 +2924,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B105" s="6">
         <v>0.75</v>
@@ -2947,7 +2947,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B106" s="6">
         <v>0.83333333333333337</v>
@@ -2970,7 +2970,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B107" s="6">
         <v>0.88888888888888884</v>
@@ -2993,7 +2993,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B108" s="6">
         <v>0.46666666666666667</v>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B109" s="6">
         <v>0.53333333333333333</v>
@@ -3039,7 +3039,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B110" s="6">
         <v>0.57777777777777772</v>
@@ -3062,7 +3062,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B111" s="6">
         <v>0.71111111111111114</v>
@@ -3091,7 +3091,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B113" s="6">
         <v>0.66666666666666663</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B114" s="6">
         <v>0.75</v>
@@ -3137,7 +3137,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B115" s="6">
         <v>0.8</v>
@@ -3160,7 +3160,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B116" s="6">
         <v>0.83333333333333337</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B117" s="6">
         <v>0.88888888888888884</v>
@@ -3206,7 +3206,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B118" s="6">
         <v>0.46666666666666667</v>
@@ -3229,7 +3229,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B119" s="6">
         <v>0.53333333333333333</v>
@@ -3252,7 +3252,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B120" s="6">
         <v>0.57777777777777772</v>
@@ -3275,7 +3275,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B121" s="6">
         <v>0.6</v>
@@ -3298,7 +3298,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B122" s="6">
         <v>0.71111111111111114</v>
@@ -3328,7 +3328,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B124" s="6">
         <v>0.66666666666666663</v>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B125" s="6">
         <v>0.71111111111111114</v>
@@ -3388,7 +3388,7 @@
     </row>
     <row r="128" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B128" s="8"/>
       <c r="E128" s="10"/>
@@ -3399,11 +3399,8 @@
       <c r="A129" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B129" s="9">
-        <v>64800</v>
-      </c>
-      <c r="C129" s="9" t="s">
-        <v>3</v>
+      <c r="B129" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="E129" s="10"/>
       <c r="F129" s="11"/>
@@ -3411,7 +3408,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B130" s="6">
         <v>0.22222222222222221</v>
@@ -3434,13 +3431,10 @@
     </row>
     <row r="131" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B131" s="9">
-        <v>32400</v>
-      </c>
-      <c r="C131" s="9" t="s">
         <v>3</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="E131" s="10"/>
       <c r="F131" s="11"/>
@@ -3448,7 +3442,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B132" s="6">
         <v>0.2</v>
@@ -3471,7 +3465,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B133" s="6">
         <v>0.24444444444444444</v>
@@ -3494,7 +3488,7 @@
     </row>
     <row r="134" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B134" s="6">
         <v>0.33333333333333331</v>
@@ -3519,11 +3513,8 @@
       <c r="A135" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B135" s="9">
-        <v>16200</v>
-      </c>
-      <c r="C135" s="9" t="s">
-        <v>3</v>
+      <c r="B135" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="E135" s="10"/>
       <c r="F135" s="11"/>
@@ -3531,7 +3522,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B136" s="6">
         <v>0.2</v>
@@ -3554,7 +3545,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B137" s="6">
         <v>0.26666666666666666</v>
@@ -3577,7 +3568,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B138" s="6">
         <v>0.33333333333333331</v>
@@ -3600,7 +3591,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B139" s="6">
         <v>0.2</v>
@@ -3623,7 +3614,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B140" s="6">
         <v>0.24444444444444444</v>

</xml_diff>

<commit_message>
updated mod cod spreadsheet
</commit_message>
<xml_diff>
--- a/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
+++ b/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13540" yWindow="1100" windowWidth="32020" windowHeight="26120" tabRatio="500"/>
+    <workbookView xWindow="18100" yWindow="1060" windowWidth="32020" windowHeight="26120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -831,7 +831,7 @@
   <dimension ref="A1:G140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,7 +875,7 @@
         <v>108</v>
       </c>
       <c r="B6" s="12">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
         <v>103</v>
@@ -948,7 +948,7 @@
       </c>
       <c r="G12" s="11">
         <f>E12/$B$6</f>
-        <v>30000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -971,7 +971,7 @@
       </c>
       <c r="G13" s="11">
         <f>E13/$B$6</f>
-        <v>40000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -994,7 +994,7 @@
       </c>
       <c r="G14" s="11">
         <f>E14/$B$6</f>
-        <v>48000</v>
+        <v>96000</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="G15" s="11">
         <f>E15/$B$6</f>
-        <v>60000</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1040,7 +1040,7 @@
       </c>
       <c r="G16" s="11">
         <f>E16/$B$6</f>
-        <v>72000</v>
+        <v>144000</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="G17" s="11">
         <f>E17/$B$6</f>
-        <v>80000</v>
+        <v>160000</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="G18" s="11">
         <f>E18/$B$6</f>
-        <v>90000</v>
+        <v>180000</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="G19" s="11">
         <f>E19/$B$6</f>
-        <v>96000</v>
+        <v>192000</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="G20" s="11">
         <f>E20/$B$6</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="G21" s="11">
         <f>E21/$B$6</f>
-        <v>106666.66666666666</v>
+        <v>213333.33333333331</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1178,7 +1178,7 @@
       </c>
       <c r="G22" s="11">
         <f>E22/$B$6</f>
-        <v>108000</v>
+        <v>216000</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="G23" s="11">
         <f>E23/$B$6</f>
-        <v>62400</v>
+        <v>124800</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1224,7 +1224,7 @@
       </c>
       <c r="G24" s="11">
         <f>E24/$B$6</f>
-        <v>54000</v>
+        <v>108000</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="G25" s="11">
         <f>E25/$B$6</f>
-        <v>66000.000000000015</v>
+        <v>132000.00000000003</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="G27" s="11">
         <f>E27/$B$6</f>
-        <v>144000</v>
+        <v>288000</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1299,7 +1299,7 @@
       </c>
       <c r="G28" s="11">
         <f>E28/$B$6</f>
-        <v>160000</v>
+        <v>320000</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1322,7 +1322,7 @@
       </c>
       <c r="G29" s="11">
         <f>E29/$B$6</f>
-        <v>180000</v>
+        <v>360000</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="G30" s="11">
         <f>E30/$B$6</f>
-        <v>200000</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="G31" s="11">
         <f>E31/$B$6</f>
-        <v>213333.33333333331</v>
+        <v>426666.66666666663</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="G32" s="11">
         <f>E32/$B$6</f>
-        <v>216000</v>
+        <v>432000</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1414,7 +1414,7 @@
       </c>
       <c r="G33" s="11">
         <f>E33/$B$6</f>
-        <v>153333.33333333331</v>
+        <v>306666.66666666663</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1437,7 +1437,7 @@
       </c>
       <c r="G34" s="11">
         <f>E34/$B$6</f>
-        <v>166666.66666666666</v>
+        <v>333333.33333333331</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1460,7 +1460,7 @@
       </c>
       <c r="G35" s="11">
         <f>E35/$B$6</f>
-        <v>173333.33333333331</v>
+        <v>346666.66666666663</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="G36" s="11">
         <f>E36/$B$6</f>
-        <v>133333.33333333334</v>
+        <v>266666.66666666669</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="G37" s="11">
         <f>E37/$B$6</f>
-        <v>138666.66666666666</v>
+        <v>277333.33333333331</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1535,7 +1535,7 @@
       </c>
       <c r="G39" s="11">
         <f>E39/$B$6</f>
-        <v>320000</v>
+        <v>640000</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1558,7 +1558,7 @@
       </c>
       <c r="G40" s="11">
         <f>E40/$B$6</f>
-        <v>360000</v>
+        <v>720000</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="G41" s="11">
         <f>E41/$B$6</f>
-        <v>384000</v>
+        <v>768000</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="G42" s="11">
         <f>E42/$B$6</f>
-        <v>400000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="G43" s="11">
         <f>E43/$B$6</f>
-        <v>426666.66666666663</v>
+        <v>853333.33333333326</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1650,7 +1650,7 @@
       </c>
       <c r="G44" s="11">
         <f>E44/$B$6</f>
-        <v>432000</v>
+        <v>864000</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="G45" s="11">
         <f>E45/$B$6</f>
-        <v>277333.33333333331</v>
+        <v>554666.66666666663</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1696,7 +1696,7 @@
       </c>
       <c r="G46" s="11">
         <f>E46/$B$6</f>
-        <v>288000</v>
+        <v>576000</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1719,7 +1719,7 @@
       </c>
       <c r="G47" s="11">
         <f>E47/$B$6</f>
-        <v>298666.66666666669</v>
+        <v>597333.33333333337</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="G48" s="11">
         <f>E48/$B$6</f>
-        <v>306666.66666666663</v>
+        <v>613333.33333333326</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="G49" s="11">
         <f>E49/$B$6</f>
-        <v>333333.33333333331</v>
+        <v>666666.66666666663</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1788,7 +1788,7 @@
       </c>
       <c r="G50" s="11">
         <f>E50/$B$6</f>
-        <v>346666.66666666663</v>
+        <v>693333.33333333326</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="G51" s="11">
         <f>E51/$B$6</f>
-        <v>373333.33333333337</v>
+        <v>746666.66666666674</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="G52" s="11">
         <f>E52/$B$6</f>
-        <v>410666.66666666663</v>
+        <v>821333.33333333326</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -1857,7 +1857,7 @@
       </c>
       <c r="G53" s="11">
         <f>E53/$B$6</f>
-        <v>266666.66666666669</v>
+        <v>533333.33333333337</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -1880,7 +1880,7 @@
       </c>
       <c r="G54" s="11">
         <f>E54/$B$6</f>
-        <v>256000</v>
+        <v>512000</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="G55" s="11">
         <f>E55/$B$6</f>
-        <v>240000</v>
+        <v>480000</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -1926,7 +1926,7 @@
       </c>
       <c r="G56" s="11">
         <f>E56/$B$6</f>
-        <v>288000</v>
+        <v>576000</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -1949,7 +1949,7 @@
       </c>
       <c r="G57" s="11">
         <f>E57/$B$6</f>
-        <v>320000</v>
+        <v>640000</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="G59" s="11">
         <f>E59/$B$6</f>
-        <v>720000</v>
+        <v>1440000</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -2002,7 +2002,7 @@
       </c>
       <c r="G60" s="11">
         <f>E60/$B$6</f>
-        <v>768000</v>
+        <v>1536000</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -2025,7 +2025,7 @@
       </c>
       <c r="G61" s="11">
         <f>E61/$B$6</f>
-        <v>800000</v>
+        <v>1600000</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -2048,7 +2048,7 @@
       </c>
       <c r="G62" s="11">
         <f>E62/$B$6</f>
-        <v>853333.33333333326</v>
+        <v>1706666.6666666665</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="G63" s="11">
         <f>E63/$B$6</f>
-        <v>864000</v>
+        <v>1728000</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -2094,7 +2094,7 @@
       </c>
       <c r="G64" s="11">
         <f>E64/$B$6</f>
-        <v>682666.66666666674</v>
+        <v>1365333.3333333335</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -2117,7 +2117,7 @@
       </c>
       <c r="G65" s="11">
         <f>E65/$B$6</f>
-        <v>704000</v>
+        <v>1408000</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -2140,7 +2140,7 @@
       </c>
       <c r="G66" s="11">
         <f>E66/$B$6</f>
-        <v>746666.66666666674</v>
+        <v>1493333.3333333335</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -2163,7 +2163,7 @@
       </c>
       <c r="G67" s="11">
         <f>E67/$B$6</f>
-        <v>640000</v>
+        <v>1280000</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -2193,7 +2193,7 @@
       </c>
       <c r="G69" s="11">
         <f>E69/$B$6</f>
-        <v>1408000</v>
+        <v>2816000</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="G70" s="11">
         <f>E70/$B$6</f>
-        <v>1493333.3333333335</v>
+        <v>2986666.666666667</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -2239,7 +2239,7 @@
       </c>
       <c r="G71" s="11">
         <f>E71/$B$6</f>
-        <v>1536000</v>
+        <v>3072000</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -2262,7 +2262,7 @@
       </c>
       <c r="G72" s="11">
         <f>E72/$B$6</f>
-        <v>1600000</v>
+        <v>3200000</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="G73" s="11">
         <f>E73/$B$6</f>
-        <v>1365333.3333333335</v>
+        <v>2730666.666666667</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -2315,7 +2315,7 @@
       </c>
       <c r="G75" s="11">
         <f>E75/$B$6</f>
-        <v>2880000</v>
+        <v>5760000</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="G76" s="11">
         <f>E76/$B$6</f>
-        <v>2986666.666666667</v>
+        <v>5973333.333333334</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="G77" s="11">
         <f>E77/$B$6</f>
-        <v>5461333.333333334</v>
+        <v>10922666.666666668</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -2384,7 +2384,7 @@
       </c>
       <c r="G78" s="11">
         <f>E78/$B$6</f>
-        <v>5760000</v>
+        <v>11520000</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -2407,7 +2407,7 @@
       </c>
       <c r="G79" s="11">
         <f>E79/$B$6</f>
-        <v>4949333.333333334</v>
+        <v>9898666.6666666679</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -2430,7 +2430,7 @@
       </c>
       <c r="G80" s="11">
         <f>E80/$B$6</f>
-        <v>5120000</v>
+        <v>10240000</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="G81" s="11">
         <f>E81/$B$6</f>
-        <v>5290666.666666667</v>
+        <v>10581333.333333334</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -2476,7 +2476,7 @@
       </c>
       <c r="G82" s="11">
         <f>E82/$B$6</f>
-        <v>5632000</v>
+        <v>11264000</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="G86" s="11">
         <f>E86/$B$6</f>
-        <v>30000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="G87" s="11">
         <f>E87/$B$6</f>
-        <v>40000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="G88" s="11">
         <f>E88/$B$6</f>
-        <v>48000</v>
+        <v>96000</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -2591,7 +2591,7 @@
       </c>
       <c r="G89" s="11">
         <f>E89/$B$6</f>
-        <v>60000</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -2614,7 +2614,7 @@
       </c>
       <c r="G90" s="11">
         <f>E90/$B$6</f>
-        <v>72000</v>
+        <v>144000</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -2637,7 +2637,7 @@
       </c>
       <c r="G91" s="11">
         <f>E91/$B$6</f>
-        <v>80000</v>
+        <v>160000</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -2660,7 +2660,7 @@
       </c>
       <c r="G92" s="11">
         <f>E92/$B$6</f>
-        <v>90000</v>
+        <v>180000</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -2683,7 +2683,7 @@
       </c>
       <c r="G93" s="11">
         <f>E93/$B$6</f>
-        <v>96000</v>
+        <v>192000</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -2706,7 +2706,7 @@
       </c>
       <c r="G94" s="11">
         <f>E94/$B$6</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="G95" s="11">
         <f>E95/$B$6</f>
-        <v>106666.66666666666</v>
+        <v>213333.33333333331</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -2752,7 +2752,7 @@
       </c>
       <c r="G96" s="11">
         <f>E96/$B$6</f>
-        <v>29333.333333333328</v>
+        <v>58666.666666666657</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="G97" s="11">
         <f>E97/$B$6</f>
-        <v>32000</v>
+        <v>64000</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="G98" s="11">
         <f>E98/$B$6</f>
-        <v>37333.333333333336</v>
+        <v>74666.666666666672</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="G99" s="11">
         <f>E99/$B$6</f>
-        <v>56000</v>
+        <v>112000</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -2844,7 +2844,7 @@
       </c>
       <c r="G100" s="11">
         <f>E100/$B$6</f>
-        <v>64000</v>
+        <v>128000</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -2867,7 +2867,7 @@
       </c>
       <c r="G101" s="11">
         <f>E101/$B$6</f>
-        <v>85333.333333333343</v>
+        <v>170666.66666666669</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="G103" s="11">
         <f>E103/$B$6</f>
-        <v>144000</v>
+        <v>288000</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
@@ -2919,7 +2919,7 @@
       </c>
       <c r="G104" s="11">
         <f>E104/$B$6</f>
-        <v>160000</v>
+        <v>320000</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
@@ -2942,7 +2942,7 @@
       </c>
       <c r="G105" s="11">
         <f>E105/$B$6</f>
-        <v>180000</v>
+        <v>360000</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
@@ -2965,7 +2965,7 @@
       </c>
       <c r="G106" s="11">
         <f>E106/$B$6</f>
-        <v>200000</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
@@ -2988,7 +2988,7 @@
       </c>
       <c r="G107" s="11">
         <f>E107/$B$6</f>
-        <v>213333.33333333331</v>
+        <v>426666.66666666663</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
@@ -3011,7 +3011,7 @@
       </c>
       <c r="G108" s="11">
         <f>E108/$B$6</f>
-        <v>112000</v>
+        <v>224000</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
@@ -3034,7 +3034,7 @@
       </c>
       <c r="G109" s="11">
         <f>E109/$B$6</f>
-        <v>128000</v>
+        <v>256000</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="G110" s="11">
         <f>E110/$B$6</f>
-        <v>138666.66666666666</v>
+        <v>277333.33333333331</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
@@ -3080,7 +3080,7 @@
       </c>
       <c r="G111" s="11">
         <f>E111/$B$6</f>
-        <v>170666.66666666669</v>
+        <v>341333.33333333337</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
@@ -3109,7 +3109,7 @@
       </c>
       <c r="G113" s="11">
         <f>E113/$B$6</f>
-        <v>320000</v>
+        <v>640000</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
@@ -3132,7 +3132,7 @@
       </c>
       <c r="G114" s="11">
         <f>E114/$B$6</f>
-        <v>360000</v>
+        <v>720000</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
@@ -3155,7 +3155,7 @@
       </c>
       <c r="G115" s="11">
         <f>E115/$B$6</f>
-        <v>384000</v>
+        <v>768000</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
@@ -3178,7 +3178,7 @@
       </c>
       <c r="G116" s="11">
         <f>E116/$B$6</f>
-        <v>400000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="G117" s="11">
         <f>E117/$B$6</f>
-        <v>426666.66666666663</v>
+        <v>853333.33333333326</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
@@ -3224,7 +3224,7 @@
       </c>
       <c r="G118" s="11">
         <f>E118/$B$6</f>
-        <v>224000</v>
+        <v>448000</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
@@ -3247,7 +3247,7 @@
       </c>
       <c r="G119" s="11">
         <f>E119/$B$6</f>
-        <v>256000</v>
+        <v>512000</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
@@ -3270,7 +3270,7 @@
       </c>
       <c r="G120" s="11">
         <f>E120/$B$6</f>
-        <v>277333.33333333331</v>
+        <v>554666.66666666663</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
@@ -3293,7 +3293,7 @@
       </c>
       <c r="G121" s="11">
         <f>E121/$B$6</f>
-        <v>288000</v>
+        <v>576000</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
@@ -3316,7 +3316,7 @@
       </c>
       <c r="G122" s="11">
         <f>E122/$B$6</f>
-        <v>341333.33333333337</v>
+        <v>682666.66666666674</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
@@ -3346,7 +3346,7 @@
       </c>
       <c r="G124" s="11">
         <f>E124/$B$6</f>
-        <v>640000</v>
+        <v>1280000</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
@@ -3369,7 +3369,7 @@
       </c>
       <c r="G125" s="11">
         <f>E125/$B$6</f>
-        <v>682666.66666666674</v>
+        <v>1365333.3333333335</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
@@ -3426,7 +3426,7 @@
       </c>
       <c r="G130" s="11">
         <f>E130/$B$6</f>
-        <v>26666.666666666664</v>
+        <v>53333.333333333328</v>
       </c>
     </row>
     <row r="131" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3460,7 +3460,7 @@
       </c>
       <c r="G132" s="11">
         <f>E132/$B$6</f>
-        <v>12000</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
@@ -3483,7 +3483,7 @@
       </c>
       <c r="G133" s="11">
         <f>E133/$B$6</f>
-        <v>14666.666666666664</v>
+        <v>29333.333333333328</v>
       </c>
     </row>
     <row r="134" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -3506,7 +3506,7 @@
       </c>
       <c r="G134" s="11">
         <f>E134/$B$6</f>
-        <v>20000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="135" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="G136" s="11">
         <f>E136/$B$6</f>
-        <v>12000</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="G137" s="11">
         <f>E137/$B$6</f>
-        <v>16000</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="G138" s="11">
         <f>E138/$B$6</f>
-        <v>20000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
@@ -3609,7 +3609,7 @@
       </c>
       <c r="G139" s="11">
         <f>E139/$B$6</f>
-        <v>12000</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
@@ -3632,7 +3632,7 @@
       </c>
       <c r="G140" s="11">
         <f>E140/$B$6</f>
-        <v>14666.666666666664</v>
+        <v>29333.333333333328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed baud rate from 6Mbaud to 8Mbaud to see if equations worked again
they work now! equations no longer getting mangled by microsoft excel.
We suspect when the sheet was edited with LibreOffice that a keyword
was not working as intended. Thank you Dr. MPEG for troubleshooting
this problem!
</commit_message>
<xml_diff>
--- a/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
+++ b/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -788,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="F139" sqref="F139"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,8 +839,8 @@
         <v>7</v>
       </c>
       <c r="B7" s="3">
-        <f>6*10^6</f>
-        <v>6000000</v>
+        <f>8*10^6</f>
+        <v>8000000</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
@@ -900,19 +899,19 @@
       </c>
       <c r="E12" s="7">
         <f>$B$7/($B$11/D12+90+ROUNDUP(($B$11/D12/90/16-1),0)*0)*($B$11*(B12)-(16*12)-80)</f>
-        <v>2941458.9104339797</v>
+        <v>3921945.2139119729</v>
       </c>
       <c r="F12" s="7">
         <f>$B$7/($B$11/D12+90+ROUNDUP(($B$11/D12/90/16-1),0)*36)*($B$11*(B12)-(16*12)-80)</f>
-        <v>2871462.0515594012</v>
+        <v>3828616.0687458687</v>
       </c>
       <c r="G12" s="8">
         <f t="shared" ref="G12:G25" si="0">E12/$B$5</f>
-        <v>588.29178208679593</v>
+        <v>784.38904278239454</v>
       </c>
       <c r="H12" s="8">
         <f t="shared" ref="H12:H25" si="1">E12/$B$6</f>
-        <v>29414.589104339797</v>
+        <v>39219.452139119727</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -927,19 +926,19 @@
       </c>
       <c r="E13" s="7">
         <f>$B$7/($B$11/D13+90+ROUNDUP(($B$11/D13/90/16-1),0)*0)*($B$11*(B13)-(16*12)-80)</f>
-        <v>3938688.8273314829</v>
+        <v>5251585.1031086436</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" ref="F13:F76" si="2">$B$7/($B$11/D13+90+ROUNDUP(($B$11/D13/90/16-1),0)*36)*($B$11*(B13)-(16*12)-80)</f>
-        <v>3844961.2403100734</v>
+        <v>5126614.9870800981</v>
       </c>
       <c r="G13" s="8">
         <f t="shared" si="0"/>
-        <v>787.73776546629654</v>
+        <v>1050.3170206217287</v>
       </c>
       <c r="H13" s="8">
         <f t="shared" si="1"/>
-        <v>39386.888273314828</v>
+        <v>52515.851031086437</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -954,19 +953,19 @@
       </c>
       <c r="E14" s="7">
         <f>$B$7/($B$11/D14+90+ROUNDUP(($B$11/D14/90/16-1),0)*0)*($B$11*(B14)-(16*12)-80)</f>
-        <v>4736472.7608494926</v>
+        <v>6315297.0144659895</v>
       </c>
       <c r="F14" s="7">
         <f t="shared" si="2"/>
-        <v>4623760.5913106184</v>
+        <v>6165014.1217474909</v>
       </c>
       <c r="G14" s="8">
         <f t="shared" si="0"/>
-        <v>947.29455216989857</v>
+        <v>1263.059402893198</v>
       </c>
       <c r="H14" s="8">
         <f t="shared" si="1"/>
-        <v>47364.727608494926</v>
+        <v>63152.970144659892</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -981,19 +980,19 @@
       </c>
       <c r="E15" s="7">
         <f>$B$7/($B$11/D15+90+ROUNDUP(($B$11/D15/90/16-1),0)*0)*($B$11*(B15)-(16*12)-80)</f>
-        <v>5933148.6611265009</v>
+        <v>7910864.8815020006</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="2"/>
-        <v>5791959.6178114293</v>
+        <v>7722612.8237485727</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" si="0"/>
-        <v>1186.6297322253001</v>
+        <v>1582.1729763004</v>
       </c>
       <c r="H15" s="8">
         <f t="shared" si="1"/>
-        <v>59331.486611265012</v>
+        <v>79108.648815020002</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1007,20 +1006,20 @@
         <v>2</v>
       </c>
       <c r="E16" s="7">
-        <f t="shared" ref="E13:E76" si="3">$B$7/($B$11/D16+90+ROUNDUP(($B$11/D16/90/16-1),0)*0)*($B$11*(B16)-(16*12)-80)</f>
-        <v>7129824.5614035092</v>
+        <f t="shared" ref="E16:E76" si="3">$B$7/($B$11/D16+90+ROUNDUP(($B$11/D16/90/16-1),0)*0)*($B$11*(B16)-(16*12)-80)</f>
+        <v>9506432.7485380117</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="2"/>
-        <v>6960158.6443122411</v>
+        <v>9280211.5257496554</v>
       </c>
       <c r="G16" s="8">
         <f t="shared" si="0"/>
-        <v>1425.9649122807018</v>
+        <v>1901.2865497076023</v>
       </c>
       <c r="H16" s="8">
         <f t="shared" si="1"/>
-        <v>71298.245614035099</v>
+        <v>95064.327485380112</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1035,19 +1034,19 @@
       </c>
       <c r="E17" s="7">
         <f t="shared" si="3"/>
-        <v>7927608.4949215185</v>
+        <v>10570144.659895359</v>
       </c>
       <c r="F17" s="7">
         <f t="shared" si="2"/>
-        <v>7738957.9953127857</v>
+        <v>10318610.660417048</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" si="0"/>
-        <v>1585.5216989843036</v>
+        <v>2114.0289319790718</v>
       </c>
       <c r="H17" s="8">
         <f t="shared" si="1"/>
-        <v>79276.08494921519</v>
+        <v>105701.44659895358</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1062,19 +1061,19 @@
       </c>
       <c r="E18" s="7">
         <f t="shared" si="3"/>
-        <v>8924838.4118190221</v>
+        <v>11899784.549092028</v>
       </c>
       <c r="F18" s="7">
         <f t="shared" si="2"/>
-        <v>8712457.184063457</v>
+        <v>11616609.578751277</v>
       </c>
       <c r="G18" s="8">
         <f t="shared" si="0"/>
-        <v>1784.9676823638044</v>
+        <v>2379.9569098184056</v>
       </c>
       <c r="H18" s="8">
         <f t="shared" si="1"/>
-        <v>89248.384118190224</v>
+        <v>118997.84549092028</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1089,19 +1088,19 @@
       </c>
       <c r="E19" s="7">
         <f t="shared" si="3"/>
-        <v>9523176.3619575258</v>
+        <v>12697568.482610034</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="2"/>
-        <v>9296556.6973138638</v>
+        <v>12395408.929751817</v>
       </c>
       <c r="G19" s="8">
         <f t="shared" si="0"/>
-        <v>1904.6352723915052</v>
+        <v>2539.5136965220067</v>
       </c>
       <c r="H19" s="8">
         <f t="shared" si="1"/>
-        <v>95231.763619575257</v>
+        <v>126975.68482610033</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1116,19 +1115,19 @@
       </c>
       <c r="E20" s="7">
         <f t="shared" si="3"/>
-        <v>9922068.3287165239</v>
+        <v>13229424.4382887</v>
       </c>
       <c r="F20" s="7">
         <f t="shared" si="2"/>
-        <v>9685956.37281413</v>
+        <v>12914608.497085506</v>
       </c>
       <c r="G20" s="8">
         <f t="shared" si="0"/>
-        <v>1984.4136657433048</v>
+        <v>2645.8848876577399</v>
       </c>
       <c r="H20" s="8">
         <f t="shared" si="1"/>
-        <v>99220.683287165244</v>
+        <v>132294.244382887</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1143,19 +1142,19 @@
       </c>
       <c r="E21" s="7">
         <f t="shared" si="3"/>
-        <v>10586888.273314869</v>
+        <v>14115851.03108649</v>
       </c>
       <c r="F21" s="7">
         <f t="shared" si="2"/>
-        <v>10334955.831981253</v>
+        <v>13779941.109308336</v>
       </c>
       <c r="G21" s="8">
         <f t="shared" si="0"/>
-        <v>2117.3776546629738</v>
+        <v>2823.1702062172981</v>
       </c>
       <c r="H21" s="8">
         <f t="shared" si="1"/>
-        <v>105868.8827331487</v>
+        <v>141158.51031086489</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1170,19 +1169,19 @@
       </c>
       <c r="E22" s="7">
         <f t="shared" si="3"/>
-        <v>10719852.262234535</v>
+        <v>14293136.349646045</v>
       </c>
       <c r="F22" s="7">
         <f t="shared" si="2"/>
-        <v>10464755.723814674</v>
+        <v>13953007.631752899</v>
       </c>
       <c r="G22" s="8">
         <f t="shared" si="0"/>
-        <v>2143.9704524469071</v>
+        <v>2858.627269929209</v>
       </c>
       <c r="H22" s="8">
         <f t="shared" si="1"/>
-        <v>107198.52262234535</v>
+        <v>142931.36349646046</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1197,19 +1196,19 @@
       </c>
       <c r="E23" s="7">
         <f t="shared" si="3"/>
-        <v>3406832.8716528174</v>
+        <v>4542443.8288704231</v>
       </c>
       <c r="F23" s="7">
         <f t="shared" si="2"/>
-        <v>3325761.6729763844</v>
+        <v>4434348.8973018462</v>
       </c>
       <c r="G23" s="8">
         <f t="shared" si="0"/>
-        <v>681.36657433056348</v>
+        <v>908.48876577408464</v>
       </c>
       <c r="H23" s="8">
         <f t="shared" si="1"/>
-        <v>34068.328716528173</v>
+        <v>45424.43828870423</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1224,19 +1223,19 @@
       </c>
       <c r="E24" s="7">
         <f t="shared" si="3"/>
-        <v>5334810.7109879963</v>
+        <v>7113080.9479839951</v>
       </c>
       <c r="F24" s="7">
         <f t="shared" si="2"/>
-        <v>5207860.1045610234</v>
+        <v>6943813.4727480318</v>
       </c>
       <c r="G24" s="8">
         <f t="shared" si="0"/>
-        <v>1066.9621421975992</v>
+        <v>1422.6161895967989</v>
       </c>
       <c r="H24" s="8">
         <f t="shared" si="1"/>
-        <v>53348.107109879966</v>
+        <v>71130.809479839954</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1251,19 +1250,19 @@
       </c>
       <c r="E25" s="7">
         <f t="shared" si="3"/>
-        <v>6531486.6112650055</v>
+        <v>8708648.8150200062</v>
       </c>
       <c r="F25" s="7">
         <f t="shared" si="2"/>
-        <v>6376059.1310618352</v>
+        <v>8501412.1747491136</v>
       </c>
       <c r="G25" s="8">
         <f t="shared" si="0"/>
-        <v>1306.2973222530011</v>
+        <v>1741.7297630040011</v>
       </c>
       <c r="H25" s="8">
         <f t="shared" si="1"/>
-        <v>65314.866112650052</v>
+        <v>87086.488150200064</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1285,19 +1284,19 @@
       </c>
       <c r="E27" s="7">
         <f t="shared" si="3"/>
-        <v>10679944.674965421</v>
+        <v>14239926.233287228</v>
       </c>
       <c r="F27" s="7">
         <f t="shared" si="2"/>
-        <v>10437415.517707488</v>
+        <v>13916554.023609987</v>
       </c>
       <c r="G27" s="8">
         <f t="shared" ref="G27:G37" si="4">E27/$B$5</f>
-        <v>2135.9889349930841</v>
+        <v>2847.9852466574457</v>
       </c>
       <c r="H27" s="8">
         <f t="shared" ref="H27:H37" si="5">E27/$B$6</f>
-        <v>106799.44674965421</v>
+        <v>142399.26233287228</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1312,19 +1311,19 @@
       </c>
       <c r="E28" s="7">
         <f t="shared" si="3"/>
-        <v>11874965.421853393</v>
+        <v>15833287.22913786</v>
       </c>
       <c r="F28" s="7">
         <f t="shared" si="2"/>
-        <v>11605298.729386326</v>
+        <v>15473731.63918177</v>
       </c>
       <c r="G28" s="8">
         <f t="shared" si="4"/>
-        <v>2374.9930843706788</v>
+        <v>3166.6574458275722</v>
       </c>
       <c r="H28" s="8">
         <f t="shared" si="5"/>
-        <v>118749.65421853393</v>
+        <v>158332.87229137859</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1339,19 +1338,19 @@
       </c>
       <c r="E29" s="7">
         <f t="shared" si="3"/>
-        <v>13368741.355463346</v>
+        <v>17824988.473951131</v>
       </c>
       <c r="F29" s="7">
         <f t="shared" si="2"/>
-        <v>13065152.743984861</v>
+        <v>17420203.658646483</v>
       </c>
       <c r="G29" s="8">
         <f t="shared" si="4"/>
-        <v>2673.7482710926693</v>
+        <v>3564.9976947902264</v>
       </c>
       <c r="H29" s="8">
         <f t="shared" si="5"/>
-        <v>133687.41355463347</v>
+        <v>178249.8847395113</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1366,19 +1365,19 @@
       </c>
       <c r="E30" s="7">
         <f t="shared" si="3"/>
-        <v>14862517.2890733</v>
+        <v>19816689.718764398</v>
       </c>
       <c r="F30" s="7">
         <f t="shared" si="2"/>
-        <v>14525006.758583395</v>
+        <v>19366675.678111196</v>
       </c>
       <c r="G30" s="8">
         <f t="shared" si="4"/>
-        <v>2972.5034578146601</v>
+        <v>3963.3379437528797</v>
       </c>
       <c r="H30" s="8">
         <f t="shared" si="5"/>
-        <v>148625.172890733</v>
+        <v>198166.89718764398</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1393,19 +1392,19 @@
       </c>
       <c r="E31" s="7">
         <f t="shared" si="3"/>
-        <v>15858367.911479946</v>
+        <v>21144490.548639927</v>
       </c>
       <c r="F31" s="7">
         <f t="shared" si="2"/>
-        <v>15498242.768315762</v>
+        <v>20664323.691087686</v>
       </c>
       <c r="G31" s="8">
         <f t="shared" si="4"/>
-        <v>3171.673582295989</v>
+        <v>4228.8981097279857</v>
       </c>
       <c r="H31" s="8">
         <f t="shared" si="5"/>
-        <v>158583.67911479945</v>
+        <v>211444.90548639928</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1420,19 +1419,19 @@
       </c>
       <c r="E32" s="7">
         <f t="shared" si="3"/>
-        <v>16057538.035961272</v>
+        <v>21410050.714615028</v>
       </c>
       <c r="F32" s="7">
         <f t="shared" si="2"/>
-        <v>15692889.970262233</v>
+        <v>20923853.293682978</v>
       </c>
       <c r="G32" s="8">
         <f t="shared" si="4"/>
-        <v>3211.5076071922545</v>
+        <v>4282.0101429230053</v>
       </c>
       <c r="H32" s="8">
         <f t="shared" si="5"/>
-        <v>160575.38035961273</v>
+        <v>214100.50714615028</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1447,19 +1446,19 @@
       </c>
       <c r="E33" s="7">
         <f t="shared" si="3"/>
-        <v>11377040.11065007</v>
+        <v>15169386.814200094</v>
       </c>
       <c r="F33" s="7">
         <f t="shared" si="2"/>
-        <v>11118680.724520143</v>
+        <v>14824907.632693525</v>
       </c>
       <c r="G33" s="8">
         <f t="shared" si="4"/>
-        <v>2275.4080221300142</v>
+        <v>3033.8773628400186</v>
       </c>
       <c r="H33" s="8">
         <f t="shared" si="5"/>
-        <v>113770.40110650071</v>
+        <v>151693.86814200095</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1474,19 +1473,19 @@
       </c>
       <c r="E34" s="7">
         <f t="shared" si="3"/>
-        <v>12372890.7330567</v>
+        <v>16497187.6440756</v>
       </c>
       <c r="F34" s="7">
         <f t="shared" si="2"/>
-        <v>12091916.734252492</v>
+        <v>16122555.645669991</v>
       </c>
       <c r="G34" s="8">
         <f t="shared" si="4"/>
-        <v>2474.5781466113399</v>
+        <v>3299.43752881512</v>
       </c>
       <c r="H34" s="8">
         <f t="shared" si="5"/>
-        <v>123728.907330567</v>
+        <v>164971.87644075599</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1501,19 +1500,19 @@
       </c>
       <c r="E35" s="7">
         <f t="shared" si="3"/>
-        <v>12870816.044260023</v>
+        <v>17161088.059013363</v>
       </c>
       <c r="F35" s="7">
         <f t="shared" si="2"/>
-        <v>12578534.739118677</v>
+        <v>16771379.652158236</v>
       </c>
       <c r="G35" s="8">
         <f t="shared" si="4"/>
-        <v>2574.1632088520046</v>
+        <v>3432.2176118026728</v>
       </c>
       <c r="H35" s="8">
         <f t="shared" si="5"/>
-        <v>128708.16044260023</v>
+        <v>171610.88059013363</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1528,19 +1527,19 @@
       </c>
       <c r="E36" s="7">
         <f t="shared" si="3"/>
-        <v>9883264.1770401187</v>
+        <v>13177685.569386825</v>
       </c>
       <c r="F36" s="7">
         <f t="shared" si="2"/>
-        <v>9658826.7099216077</v>
+        <v>12878435.613228813</v>
       </c>
       <c r="G36" s="8">
         <f t="shared" si="4"/>
-        <v>1976.6528354080237</v>
+        <v>2635.5371138773648</v>
       </c>
       <c r="H36" s="8">
         <f t="shared" si="5"/>
-        <v>98832.641770401184</v>
+        <v>131776.85569386824</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1555,19 +1554,19 @@
       </c>
       <c r="E37" s="7">
         <f t="shared" si="3"/>
-        <v>10281604.426002767</v>
+        <v>13708805.901337024</v>
       </c>
       <c r="F37" s="7">
         <f t="shared" si="2"/>
-        <v>10048121.113814546</v>
+        <v>13397494.818419397</v>
       </c>
       <c r="G37" s="8">
         <f t="shared" si="4"/>
-        <v>2056.3208852005532</v>
+        <v>2741.7611802674046</v>
       </c>
       <c r="H37" s="8">
         <f t="shared" si="5"/>
-        <v>102816.04426002767</v>
+        <v>137088.05901337025</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1589,19 +1588,19 @@
       </c>
       <c r="E39" s="7">
         <f t="shared" si="3"/>
-        <v>15811418.047882145</v>
+        <v>21081890.730509527</v>
       </c>
       <c r="F39" s="7">
         <f t="shared" si="2"/>
-        <v>15436174.038115792</v>
+        <v>20581565.384154391</v>
       </c>
       <c r="G39" s="8">
         <f t="shared" ref="G39:G57" si="6">E39/$B$5</f>
-        <v>3162.2836095764292</v>
+        <v>4216.3781461019053</v>
       </c>
       <c r="H39" s="8">
         <f t="shared" ref="H39:H57" si="7">E39/$B$6</f>
-        <v>158114.18047882145</v>
+        <v>210818.90730509526</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1616,19 +1615,19 @@
       </c>
       <c r="E40" s="7">
         <f t="shared" si="3"/>
-        <v>17800368.32412523</v>
+        <v>23733824.432166975</v>
       </c>
       <c r="F40" s="7">
         <f t="shared" si="2"/>
-        <v>17377921.610931318</v>
+        <v>23170562.147908427</v>
       </c>
       <c r="G40" s="8">
         <f t="shared" si="6"/>
-        <v>3560.0736648250459</v>
+        <v>4746.7648864333951</v>
       </c>
       <c r="H40" s="8">
         <f t="shared" si="7"/>
-        <v>178003.68324125229</v>
+        <v>237338.24432166974</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1643,19 +1642,19 @@
       </c>
       <c r="E41" s="7">
         <f t="shared" si="3"/>
-        <v>18993738.489871088</v>
+        <v>25324984.653161451</v>
       </c>
       <c r="F41" s="7">
         <f t="shared" si="2"/>
-        <v>18542970.15462064</v>
+        <v>24723960.206160855</v>
       </c>
       <c r="G41" s="8">
         <f t="shared" si="6"/>
-        <v>3798.7476979742178</v>
+        <v>5064.9969306322901</v>
       </c>
       <c r="H41" s="8">
         <f t="shared" si="7"/>
-        <v>189937.38489871088</v>
+        <v>253249.84653161452</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1670,19 +1669,19 @@
       </c>
       <c r="E42" s="7">
         <f t="shared" si="3"/>
-        <v>19789318.600368317</v>
+        <v>26385758.133824423</v>
       </c>
       <c r="F42" s="7">
         <f t="shared" si="2"/>
-        <v>19319669.183746845</v>
+        <v>25759558.911662463</v>
       </c>
       <c r="G42" s="8">
         <f t="shared" si="6"/>
-        <v>3957.8637200736634</v>
+        <v>5277.1516267648849</v>
       </c>
       <c r="H42" s="8">
         <f t="shared" si="7"/>
-        <v>197893.18600368316</v>
+        <v>263857.58133824426</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1697,19 +1696,19 @@
       </c>
       <c r="E43" s="7">
         <f t="shared" si="3"/>
-        <v>21115285.451197058</v>
+        <v>28153713.934929408</v>
       </c>
       <c r="F43" s="7">
         <f t="shared" si="2"/>
-        <v>20614167.565623879</v>
+        <v>27485556.754165173</v>
       </c>
       <c r="G43" s="8">
         <f t="shared" si="6"/>
-        <v>4223.057090239412</v>
+        <v>5630.742786985882</v>
       </c>
       <c r="H43" s="8">
         <f t="shared" si="7"/>
-        <v>211152.85451197057</v>
+        <v>281537.13934929407</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1724,19 +1723,19 @@
       </c>
       <c r="E44" s="7">
         <f t="shared" si="3"/>
-        <v>21380478.821362801</v>
+        <v>28507305.0951504</v>
       </c>
       <c r="F44" s="7">
         <f t="shared" si="2"/>
-        <v>20873067.24199928</v>
+        <v>27830756.32266571</v>
       </c>
       <c r="G44" s="8">
         <f t="shared" si="6"/>
-        <v>4276.0957642725598</v>
+        <v>5701.46101903008</v>
       </c>
       <c r="H44" s="8">
         <f t="shared" si="7"/>
-        <v>213804.78821362799</v>
+        <v>285073.05095150397</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1751,19 +1750,19 @@
       </c>
       <c r="E45" s="7">
         <f t="shared" si="3"/>
-        <v>13689871.086556172</v>
+        <v>18253161.448741563</v>
       </c>
       <c r="F45" s="7">
         <f t="shared" si="2"/>
-        <v>13364976.627112551</v>
+        <v>17819968.836150069</v>
       </c>
       <c r="G45" s="8">
         <f t="shared" si="6"/>
-        <v>2737.9742173112345</v>
+        <v>3650.6322897483124</v>
       </c>
       <c r="H45" s="8">
         <f t="shared" si="7"/>
-        <v>136898.71086556173</v>
+        <v>182531.61448741562</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1778,19 +1777,19 @@
       </c>
       <c r="E46" s="7">
         <f t="shared" si="3"/>
-        <v>14220257.826887662</v>
+        <v>18960343.76918355</v>
       </c>
       <c r="F46" s="7">
         <f t="shared" si="2"/>
-        <v>13882775.979863357</v>
+        <v>18510367.973151144</v>
       </c>
       <c r="G46" s="8">
         <f t="shared" si="6"/>
-        <v>2844.0515653775324</v>
+        <v>3792.0687538367101</v>
       </c>
       <c r="H46" s="8">
         <f t="shared" si="7"/>
-        <v>142202.57826887662</v>
+        <v>189603.43769183551</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -1805,19 +1804,19 @@
       </c>
       <c r="E47" s="7">
         <f t="shared" si="3"/>
-        <v>14750644.567219147</v>
+        <v>19667526.08962553</v>
       </c>
       <c r="F47" s="7">
         <f t="shared" si="2"/>
-        <v>14400575.332614161</v>
+        <v>19200767.110152218</v>
       </c>
       <c r="G47" s="8">
         <f t="shared" si="6"/>
-        <v>2950.1289134438293</v>
+        <v>3933.5052179251061</v>
       </c>
       <c r="H47" s="8">
         <f t="shared" si="7"/>
-        <v>147506.44567219148</v>
+        <v>196675.26089625529</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -1832,19 +1831,19 @@
       </c>
       <c r="E48" s="7">
         <f t="shared" si="3"/>
-        <v>15148434.622467775</v>
+        <v>20197912.829957034</v>
       </c>
       <c r="F48" s="7">
         <f t="shared" si="2"/>
-        <v>14788924.847177276</v>
+        <v>19718566.462903038</v>
       </c>
       <c r="G48" s="8">
         <f t="shared" si="6"/>
-        <v>3029.6869244935551</v>
+        <v>4039.5825659914067</v>
       </c>
       <c r="H48" s="8">
         <f t="shared" si="7"/>
-        <v>151484.34622467775</v>
+        <v>201979.12829957035</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1859,19 +1858,19 @@
       </c>
       <c r="E49" s="7">
         <f t="shared" si="3"/>
-        <v>16474401.47329649</v>
+        <v>21965868.63106199</v>
       </c>
       <c r="F49" s="7">
         <f t="shared" si="2"/>
-        <v>16083423.229054285</v>
+        <v>21444564.305405717</v>
       </c>
       <c r="G49" s="8">
         <f t="shared" si="6"/>
-        <v>3294.8802946592978</v>
+        <v>4393.1737262123979</v>
       </c>
       <c r="H49" s="8">
         <f t="shared" si="7"/>
-        <v>164744.01473296489</v>
+        <v>219658.6863106199</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -1886,19 +1885,19 @@
       </c>
       <c r="E50" s="7">
         <f t="shared" si="3"/>
-        <v>17137384.898710862</v>
+        <v>22849846.531614482</v>
       </c>
       <c r="F50" s="7">
         <f t="shared" si="2"/>
-        <v>16730672.419992803</v>
+        <v>22307563.22665707</v>
       </c>
       <c r="G50" s="8">
         <f t="shared" si="6"/>
-        <v>3427.4769797421723</v>
+        <v>4569.969306322896</v>
       </c>
       <c r="H50" s="8">
         <f t="shared" si="7"/>
-        <v>171373.84898710862</v>
+        <v>228498.46531614484</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -1913,19 +1912,19 @@
       </c>
       <c r="E51" s="7">
         <f t="shared" si="3"/>
-        <v>18463351.749539599</v>
+        <v>24617802.332719468</v>
       </c>
       <c r="F51" s="7">
         <f t="shared" si="2"/>
-        <v>18025170.801869836</v>
+        <v>24033561.069159783</v>
       </c>
       <c r="G51" s="8">
         <f t="shared" si="6"/>
-        <v>3692.6703499079199</v>
+        <v>4923.5604665438932</v>
       </c>
       <c r="H51" s="8">
         <f t="shared" si="7"/>
-        <v>184633.51749539599</v>
+        <v>246178.02332719468</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -1940,19 +1939,19 @@
       </c>
       <c r="E52" s="7">
         <f t="shared" si="3"/>
-        <v>20319705.340699825</v>
+        <v>27092940.454266436</v>
       </c>
       <c r="F52" s="7">
         <f t="shared" si="2"/>
-        <v>19837468.536497671</v>
+        <v>26449958.048663564</v>
       </c>
       <c r="G52" s="8">
         <f t="shared" si="6"/>
-        <v>4063.941068139965</v>
+        <v>5418.5880908532872</v>
       </c>
       <c r="H52" s="8">
         <f t="shared" si="7"/>
-        <v>203197.05340699825</v>
+        <v>270929.40454266436</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -1967,19 +1966,19 @@
       </c>
       <c r="E53" s="7">
         <f t="shared" si="3"/>
-        <v>13159484.346224688</v>
+        <v>17545979.128299586</v>
       </c>
       <c r="F53" s="7">
         <f t="shared" si="2"/>
-        <v>12847177.27436175</v>
+        <v>17129569.699149001</v>
       </c>
       <c r="G53" s="8">
         <f t="shared" si="6"/>
-        <v>2631.8968692449375</v>
+        <v>3509.1958256599173</v>
       </c>
       <c r="H53" s="8">
         <f t="shared" si="7"/>
-        <v>131594.84346224688</v>
+        <v>175459.79128299587</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -1994,19 +1993,19 @@
       </c>
       <c r="E54" s="7">
         <f t="shared" si="3"/>
-        <v>12629097.605893178</v>
+        <v>16838796.807857573</v>
       </c>
       <c r="F54" s="7">
         <f t="shared" si="2"/>
-        <v>12329377.921610923</v>
+        <v>16439170.562147899</v>
       </c>
       <c r="G54" s="8">
         <f t="shared" si="6"/>
-        <v>2525.8195211786356</v>
+        <v>3367.7593615715145</v>
       </c>
       <c r="H54" s="8">
         <f t="shared" si="7"/>
-        <v>126290.97605893177</v>
+        <v>168387.96807857574</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -2021,19 +2020,19 @@
       </c>
       <c r="E55" s="7">
         <f t="shared" si="3"/>
-        <v>11833517.495395949</v>
+        <v>15778023.327194599</v>
       </c>
       <c r="F55" s="7">
         <f t="shared" si="2"/>
-        <v>11552678.892484717</v>
+        <v>15403571.85664629</v>
       </c>
       <c r="G55" s="8">
         <f t="shared" si="6"/>
-        <v>2366.7034990791899</v>
+        <v>3155.6046654389197</v>
       </c>
       <c r="H55" s="8">
         <f t="shared" si="7"/>
-        <v>118335.17495395949</v>
+        <v>157780.233271946</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -2048,19 +2047,19 @@
       </c>
       <c r="E56" s="7">
         <f t="shared" si="3"/>
-        <v>14220257.826887662</v>
+        <v>18960343.76918355</v>
       </c>
       <c r="F56" s="7">
         <f t="shared" si="2"/>
-        <v>13882775.979863357</v>
+        <v>18510367.973151144</v>
       </c>
       <c r="G56" s="8">
         <f t="shared" si="6"/>
-        <v>2844.0515653775324</v>
+        <v>3792.0687538367101</v>
       </c>
       <c r="H56" s="8">
         <f t="shared" si="7"/>
-        <v>142202.57826887662</v>
+        <v>189603.43769183551</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2075,19 +2074,19 @@
       </c>
       <c r="E57" s="7">
         <f t="shared" si="3"/>
-        <v>15811418.047882145</v>
+        <v>21081890.730509527</v>
       </c>
       <c r="F57" s="7">
         <f t="shared" si="2"/>
-        <v>15436174.038115792</v>
+        <v>20581565.384154391</v>
       </c>
       <c r="G57" s="8">
         <f t="shared" si="6"/>
-        <v>3162.2836095764292</v>
+        <v>4216.3781461019053</v>
       </c>
       <c r="H57" s="8">
         <f t="shared" si="7"/>
-        <v>158114.18047882145</v>
+        <v>210818.90730509526</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2110,19 +2109,19 @@
       </c>
       <c r="E59" s="7">
         <f t="shared" si="3"/>
-        <v>22219770.114942528</v>
+        <v>29626360.153256707</v>
       </c>
       <c r="F59" s="7">
         <f t="shared" si="2"/>
-        <v>21739991.003148898</v>
+        <v>28986654.670865197</v>
       </c>
       <c r="G59" s="8">
         <f t="shared" ref="G59:G67" si="8">E59/$B$5</f>
-        <v>4443.954022988506</v>
+        <v>5925.2720306513411</v>
       </c>
       <c r="H59" s="8">
         <f t="shared" ref="H59:H67" si="9">E59/$B$6</f>
-        <v>222197.70114942529</v>
+        <v>296263.60153256706</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2137,19 +2136,19 @@
       </c>
       <c r="E60" s="7">
         <f t="shared" si="3"/>
-        <v>23709425.287356321</v>
+        <v>31612567.049808431</v>
       </c>
       <c r="F60" s="7">
         <f t="shared" si="2"/>
-        <v>23197480.881691407</v>
+        <v>30929974.508921877</v>
       </c>
       <c r="G60" s="8">
         <f t="shared" si="8"/>
-        <v>4741.8850574712642</v>
+        <v>6322.5134099616862</v>
       </c>
       <c r="H60" s="8">
         <f t="shared" si="9"/>
-        <v>237094.25287356321</v>
+        <v>316125.67049808434</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -2164,19 +2163,19 @@
       </c>
       <c r="E61" s="7">
         <f t="shared" si="3"/>
-        <v>24702528.735632174</v>
+        <v>32936704.980842903</v>
       </c>
       <c r="F61" s="7">
         <f t="shared" si="2"/>
-        <v>24169140.800719738</v>
+        <v>32225521.067626316</v>
       </c>
       <c r="G61" s="8">
         <f t="shared" si="8"/>
-        <v>4940.5057471264345</v>
+        <v>6587.3409961685802</v>
       </c>
       <c r="H61" s="8">
         <f t="shared" si="9"/>
-        <v>247025.28735632173</v>
+        <v>329367.04980842903</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -2191,19 +2190,19 @@
       </c>
       <c r="E62" s="7">
         <f t="shared" si="3"/>
-        <v>26357701.149425291</v>
+        <v>35143601.532567054</v>
       </c>
       <c r="F62" s="7">
         <f t="shared" si="2"/>
-        <v>25788573.99910032</v>
+        <v>34384765.332133755</v>
       </c>
       <c r="G62" s="8">
         <f t="shared" si="8"/>
-        <v>5271.5402298850577</v>
+        <v>7028.7203065134108</v>
       </c>
       <c r="H62" s="8">
         <f t="shared" si="9"/>
-        <v>263577.01149425289</v>
+        <v>351436.01532567054</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -2218,19 +2217,19 @@
       </c>
       <c r="E63" s="7">
         <f t="shared" si="3"/>
-        <v>26688735.632183906</v>
+        <v>35584980.842911884</v>
       </c>
       <c r="F63" s="7">
         <f t="shared" si="2"/>
-        <v>26112460.638776429</v>
+        <v>34816614.185035236</v>
       </c>
       <c r="G63" s="8">
         <f t="shared" si="8"/>
-        <v>5337.7471264367814</v>
+        <v>7116.9961685823764</v>
       </c>
       <c r="H63" s="8">
         <f t="shared" si="9"/>
-        <v>266887.35632183903</v>
+        <v>355849.80842911883</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -2245,19 +2244,19 @@
       </c>
       <c r="E64" s="7">
         <f t="shared" si="3"/>
-        <v>21061149.425287351</v>
+        <v>28081532.567049805</v>
       </c>
       <c r="F64" s="7">
         <f t="shared" si="2"/>
-        <v>20606387.764282499</v>
+        <v>27475183.685709998</v>
       </c>
       <c r="G64" s="8">
         <f t="shared" si="8"/>
-        <v>4212.2298850574698</v>
+        <v>5616.3065134099606</v>
       </c>
       <c r="H64" s="8">
         <f t="shared" si="9"/>
-        <v>210611.4942528735</v>
+        <v>280815.32567049807</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2272,19 +2271,19 @@
       </c>
       <c r="E65" s="7">
         <f t="shared" si="3"/>
-        <v>21723218.390804589</v>
+        <v>28964291.187739454</v>
       </c>
       <c r="F65" s="7">
         <f t="shared" si="2"/>
-        <v>21254161.04363472</v>
+        <v>28338881.391512956</v>
       </c>
       <c r="G65" s="8">
         <f t="shared" si="8"/>
-        <v>4344.6436781609182</v>
+        <v>5792.8582375478909</v>
       </c>
       <c r="H65" s="8">
         <f t="shared" si="9"/>
-        <v>217232.18390804587</v>
+        <v>289642.91187739454</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2299,19 +2298,19 @@
       </c>
       <c r="E66" s="7">
         <f t="shared" si="3"/>
-        <v>23047356.321839087</v>
+        <v>30729808.429118786</v>
       </c>
       <c r="F66" s="7">
         <f t="shared" si="2"/>
-        <v>22549707.602339189</v>
+        <v>30066276.803118918</v>
       </c>
       <c r="G66" s="8">
         <f t="shared" si="8"/>
-        <v>4609.4712643678176</v>
+        <v>6145.9616858237569</v>
       </c>
       <c r="H66" s="8">
         <f t="shared" si="9"/>
-        <v>230473.56321839086</v>
+        <v>307298.08429118787</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2326,19 +2325,19 @@
       </c>
       <c r="E67" s="7">
         <f t="shared" si="3"/>
-        <v>19737011.494252883</v>
+        <v>26316015.325670514</v>
       </c>
       <c r="F67" s="7">
         <f t="shared" si="2"/>
-        <v>19310841.205578059</v>
+        <v>25747788.274104077</v>
       </c>
       <c r="G67" s="8">
         <f t="shared" si="8"/>
-        <v>3947.4022988505767</v>
+        <v>5263.2030651341029</v>
       </c>
       <c r="H67" s="8">
         <f t="shared" si="9"/>
-        <v>197370.11494252883</v>
+        <v>263160.15325670515</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -2361,19 +2360,19 @@
       </c>
       <c r="E69" s="7">
         <f t="shared" si="3"/>
-        <v>26031955.922865</v>
+        <v>34709274.563820004</v>
       </c>
       <c r="F69" s="7">
         <f t="shared" si="2"/>
-        <v>25443187.937533643</v>
+        <v>33924250.583378188</v>
       </c>
       <c r="G69" s="8">
         <f>E69/$B$5</f>
-        <v>5206.3911845729999</v>
+        <v>6941.8549127640008</v>
       </c>
       <c r="H69" s="8">
         <f>E69/$B$6</f>
-        <v>260319.55922865</v>
+        <v>347092.74563820002</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -2388,19 +2387,19 @@
       </c>
       <c r="E70" s="7">
         <f t="shared" si="3"/>
-        <v>27618732.782369152</v>
+        <v>36824977.043158874</v>
       </c>
       <c r="F70" s="7">
         <f t="shared" si="2"/>
-        <v>26994076.467420578</v>
+        <v>35992101.956560768</v>
       </c>
       <c r="G70" s="8">
         <f>E70/$B$5</f>
-        <v>5523.7465564738304</v>
+        <v>7364.9954086317748</v>
       </c>
       <c r="H70" s="8">
         <f>E70/$B$6</f>
-        <v>276187.32782369154</v>
+        <v>368249.77043158875</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -2415,19 +2414,19 @@
       </c>
       <c r="E71" s="7">
         <f t="shared" si="3"/>
-        <v>28412121.212121211</v>
+        <v>37882828.282828286</v>
       </c>
       <c r="F71" s="7">
         <f t="shared" si="2"/>
-        <v>27769520.732364025</v>
+        <v>37026027.643152036</v>
       </c>
       <c r="G71" s="8">
         <f>E71/$B$5</f>
-        <v>5682.424242424242</v>
+        <v>7576.5656565656573</v>
       </c>
       <c r="H71" s="8">
         <f>E71/$B$6</f>
-        <v>284121.2121212121</v>
+        <v>378828.28282828286</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2442,19 +2441,19 @@
       </c>
       <c r="E72" s="7">
         <f t="shared" si="3"/>
-        <v>29602203.856749296</v>
+        <v>39469605.142332397</v>
       </c>
       <c r="F72" s="7">
         <f t="shared" si="2"/>
-        <v>28932687.129779201</v>
+        <v>38576916.17303893</v>
       </c>
       <c r="G72" s="8">
         <f>E72/$B$5</f>
-        <v>5920.4407713498595</v>
+        <v>7893.9210284664796</v>
       </c>
       <c r="H72" s="8">
         <f>E72/$B$6</f>
-        <v>296022.03856749297</v>
+        <v>394696.05142332398</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2469,19 +2468,19 @@
       </c>
       <c r="E73" s="7">
         <f t="shared" si="3"/>
-        <v>25238567.49311294</v>
+        <v>33651423.324150592</v>
       </c>
       <c r="F73" s="7">
         <f t="shared" si="2"/>
-        <v>24667743.672590192</v>
+        <v>32890324.896786924</v>
       </c>
       <c r="G73" s="8">
         <f>E73/$B$5</f>
-        <v>5047.7134986225883</v>
+        <v>6730.2846648301183</v>
       </c>
       <c r="H73" s="8">
         <f>E73/$B$6</f>
-        <v>252385.67493112941</v>
+        <v>336514.23324150592</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -2504,19 +2503,19 @@
       </c>
       <c r="E75" s="7">
         <f t="shared" si="3"/>
-        <v>31022099.95414947</v>
+        <v>41362799.938865967</v>
       </c>
       <c r="F75" s="7">
         <f t="shared" si="2"/>
-        <v>30321412.566101998</v>
+        <v>40428550.088135995</v>
       </c>
       <c r="G75" s="8">
         <f t="shared" ref="G75:G82" si="10">E75/$B$5</f>
-        <v>6204.4199908298942</v>
+        <v>8272.5599877731929</v>
       </c>
       <c r="H75" s="8">
         <f t="shared" ref="H75:H82" si="11">E75/$B$6</f>
-        <v>310220.9995414947</v>
+        <v>413627.99938865966</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -2531,19 +2530,19 @@
       </c>
       <c r="E76" s="7">
         <f t="shared" si="3"/>
-        <v>32177533.241632286</v>
+        <v>42903377.655509718</v>
       </c>
       <c r="F76" s="7">
         <f t="shared" si="2"/>
-        <v>31450748.409070548</v>
+        <v>41934331.212094061</v>
       </c>
       <c r="G76" s="8">
         <f t="shared" si="10"/>
-        <v>6435.5066483264573</v>
+        <v>8580.6755311019442</v>
       </c>
       <c r="H76" s="8">
         <f t="shared" si="11"/>
-        <v>321775.33241632284</v>
+        <v>429033.7765550972</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -2558,19 +2557,19 @@
       </c>
       <c r="E77" s="7">
         <f t="shared" ref="E77:E140" si="12">$B$7/($B$11/D77+90+ROUNDUP(($B$11/D77/90/16-1),0)*0)*($B$11*(B77)-(16*12)-80)</f>
-        <v>33558974.358974352</v>
+        <v>44745299.145299144</v>
       </c>
       <c r="F77" s="7">
         <f t="shared" ref="F77:F140" si="13">$B$7/($B$11/D77+90+ROUNDUP(($B$11/D77/90/16-1),0)*36)*($B$11*(B77)-(16*12)-80)</f>
-        <v>32837275.985663075</v>
+        <v>43783034.647550769</v>
       </c>
       <c r="G77" s="8">
         <f t="shared" si="10"/>
-        <v>6711.7948717948702</v>
+        <v>8949.0598290598282</v>
       </c>
       <c r="H77" s="8">
         <f t="shared" si="11"/>
-        <v>335589.74358974351</v>
+        <v>447452.99145299144</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2585,19 +2584,19 @@
       </c>
       <c r="E78" s="7">
         <f t="shared" si="12"/>
-        <v>35405128.205128208</v>
+        <v>47206837.606837608</v>
       </c>
       <c r="F78" s="7">
         <f t="shared" si="13"/>
-        <v>34643727.598566309</v>
+        <v>46191636.798088409</v>
       </c>
       <c r="G78" s="8">
         <f t="shared" si="10"/>
-        <v>7081.0256410256416</v>
+        <v>9441.3675213675215</v>
       </c>
       <c r="H78" s="8">
         <f t="shared" si="11"/>
-        <v>354051.28205128206</v>
+        <v>472068.37606837606</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2612,19 +2611,19 @@
       </c>
       <c r="E79" s="7">
         <f t="shared" si="12"/>
-        <v>30394139.194139175</v>
+        <v>40525518.9255189</v>
       </c>
       <c r="F79" s="7">
         <f t="shared" si="13"/>
-        <v>29740501.792114671</v>
+        <v>39654002.389486231</v>
       </c>
       <c r="G79" s="8">
         <f t="shared" si="10"/>
-        <v>6078.827838827835</v>
+        <v>8105.10378510378</v>
       </c>
       <c r="H79" s="8">
         <f t="shared" si="11"/>
-        <v>303941.39194139175</v>
+        <v>405255.18925518898</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -2639,19 +2638,19 @@
       </c>
       <c r="E80" s="7">
         <f t="shared" si="12"/>
-        <v>31449084.249084264</v>
+        <v>41932112.332112357</v>
       </c>
       <c r="F80" s="7">
         <f t="shared" si="13"/>
-        <v>30772759.856630839</v>
+        <v>41030346.475507788</v>
       </c>
       <c r="G80" s="8">
         <f t="shared" si="10"/>
-        <v>6289.8168498168525</v>
+        <v>8386.4224664224712</v>
       </c>
       <c r="H80" s="8">
         <f t="shared" si="11"/>
-        <v>314490.84249084262</v>
+        <v>419321.1233211236</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -2666,19 +2665,19 @@
       </c>
       <c r="E81" s="7">
         <f t="shared" si="12"/>
-        <v>32504029.304029308</v>
+        <v>43338705.738705747</v>
       </c>
       <c r="F81" s="7">
         <f t="shared" si="13"/>
-        <v>31805017.921146955</v>
+        <v>42406690.561529279</v>
       </c>
       <c r="G81" s="8">
         <f t="shared" si="10"/>
-        <v>6500.8058608058618</v>
+        <v>8667.7411477411497</v>
       </c>
       <c r="H81" s="8">
         <f t="shared" si="11"/>
-        <v>325040.29304029309</v>
+        <v>433387.05738705746</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -2693,19 +2692,19 @@
       </c>
       <c r="E82" s="7">
         <f t="shared" si="12"/>
-        <v>34613919.413919397</v>
+        <v>46151892.551892534</v>
       </c>
       <c r="F82" s="7">
         <f t="shared" si="13"/>
-        <v>33869534.050179191</v>
+        <v>45159378.73357226</v>
       </c>
       <c r="G82" s="8">
         <f t="shared" si="10"/>
-        <v>6922.7838827838796</v>
+        <v>9230.3785103785067</v>
       </c>
       <c r="H82" s="8">
         <f t="shared" si="11"/>
-        <v>346139.19413919398</v>
+        <v>461518.92551892536</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -2746,19 +2745,19 @@
       </c>
       <c r="E86" s="7">
         <f t="shared" si="12"/>
-        <v>2343120.9602954756</v>
+        <v>3124161.2803939674</v>
       </c>
       <c r="F86" s="7">
         <f t="shared" si="13"/>
-        <v>2287362.5383089958</v>
+        <v>3049816.7177453279</v>
       </c>
       <c r="G86" s="8">
         <f t="shared" ref="G86:G101" si="14">E86/$B$5</f>
-        <v>468.62419205909509</v>
+        <v>624.83225607879353</v>
       </c>
       <c r="H86" s="8">
         <f t="shared" ref="H86:H101" si="15">E86/$B$6</f>
-        <v>23431.209602954754</v>
+        <v>31241.612803939675</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -2773,19 +2772,19 @@
       </c>
       <c r="E87" s="7">
         <f t="shared" si="12"/>
-        <v>3938688.8273314829</v>
+        <v>5251585.1031086436</v>
       </c>
       <c r="F87" s="7">
         <f t="shared" si="13"/>
-        <v>3844961.2403100734</v>
+        <v>5126614.9870800981</v>
       </c>
       <c r="G87" s="8">
         <f t="shared" si="14"/>
-        <v>787.73776546629654</v>
+        <v>1050.3170206217287</v>
       </c>
       <c r="H87" s="8">
         <f t="shared" si="15"/>
-        <v>39386.888273314828</v>
+        <v>52515.851031086437</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -2800,19 +2799,19 @@
       </c>
       <c r="E88" s="7">
         <f t="shared" si="12"/>
-        <v>4736472.7608494926</v>
+        <v>6315297.0144659895</v>
       </c>
       <c r="F88" s="7">
         <f t="shared" si="13"/>
-        <v>4623760.5913106184</v>
+        <v>6165014.1217474909</v>
       </c>
       <c r="G88" s="8">
         <f t="shared" si="14"/>
-        <v>947.29455216989857</v>
+        <v>1263.059402893198</v>
       </c>
       <c r="H88" s="8">
         <f t="shared" si="15"/>
-        <v>47364.727608494926</v>
+        <v>63152.970144659892</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -2827,19 +2826,19 @@
       </c>
       <c r="E89" s="7">
         <f t="shared" si="12"/>
-        <v>5268328.7165281577</v>
+        <v>7024438.28870421</v>
       </c>
       <c r="F89" s="7">
         <f t="shared" si="13"/>
-        <v>5142960.1586443065</v>
+        <v>6857280.2115257429</v>
       </c>
       <c r="G89" s="8">
         <f t="shared" si="14"/>
-        <v>1053.6657433056316</v>
+        <v>1404.8876577408421</v>
       </c>
       <c r="H89" s="8">
         <f t="shared" si="15"/>
-        <v>52683.287165281574</v>
+        <v>70244.382887042098</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -2854,19 +2853,19 @@
       </c>
       <c r="E90" s="7">
         <f t="shared" si="12"/>
-        <v>7129824.5614035092</v>
+        <v>9506432.7485380117</v>
       </c>
       <c r="F90" s="7">
         <f t="shared" si="13"/>
-        <v>6960158.6443122411</v>
+        <v>9280211.5257496554</v>
       </c>
       <c r="G90" s="8">
         <f t="shared" si="14"/>
-        <v>1425.9649122807018</v>
+        <v>1901.2865497076023</v>
       </c>
       <c r="H90" s="8">
         <f t="shared" si="15"/>
-        <v>71298.245614035099</v>
+        <v>95064.327485380112</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -2881,19 +2880,19 @@
       </c>
       <c r="E91" s="7">
         <f t="shared" si="12"/>
-        <v>7927608.4949215185</v>
+        <v>10570144.659895359</v>
       </c>
       <c r="F91" s="7">
         <f t="shared" si="13"/>
-        <v>7738957.9953127857</v>
+        <v>10318610.660417048</v>
       </c>
       <c r="G91" s="8">
         <f t="shared" si="14"/>
-        <v>1585.5216989843036</v>
+        <v>2114.0289319790718</v>
       </c>
       <c r="H91" s="8">
         <f t="shared" si="15"/>
-        <v>79276.08494921519</v>
+        <v>105701.44659895358</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -2908,19 +2907,19 @@
       </c>
       <c r="E92" s="7">
         <f t="shared" si="12"/>
-        <v>8725392.4284395166</v>
+        <v>11633856.571252689</v>
       </c>
       <c r="F92" s="7">
         <f t="shared" si="13"/>
-        <v>8517757.3463133182</v>
+        <v>11357009.795084424</v>
       </c>
       <c r="G92" s="8">
         <f t="shared" si="14"/>
-        <v>1745.0784856879034</v>
+        <v>2326.7713142505377</v>
       </c>
       <c r="H92" s="8">
         <f t="shared" si="15"/>
-        <v>87253.924284395165</v>
+        <v>116338.56571252689</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -2935,19 +2934,19 @@
       </c>
       <c r="E93" s="7">
         <f t="shared" si="12"/>
-        <v>9257248.3841181938</v>
+        <v>12342997.845490925</v>
       </c>
       <c r="F93" s="7">
         <f t="shared" si="13"/>
-        <v>9036956.9136470184</v>
+        <v>12049275.884862693</v>
       </c>
       <c r="G93" s="8">
         <f t="shared" si="14"/>
-        <v>1851.4496768236388</v>
+        <v>2468.5995690981849</v>
       </c>
       <c r="H93" s="8">
         <f t="shared" si="15"/>
-        <v>92572.483841181936</v>
+        <v>123429.97845490924</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -2962,19 +2961,19 @@
       </c>
       <c r="E94" s="7">
         <f t="shared" si="12"/>
-        <v>9789104.3397968579</v>
+        <v>13052139.119729144</v>
       </c>
       <c r="F94" s="7">
         <f t="shared" si="13"/>
-        <v>9556156.4809807073</v>
+        <v>12741541.974640943</v>
       </c>
       <c r="G94" s="8">
         <f t="shared" si="14"/>
-        <v>1957.8208679593715</v>
+        <v>2610.427823945829</v>
       </c>
       <c r="H94" s="8">
         <f t="shared" si="15"/>
-        <v>97891.043397968577</v>
+        <v>130521.39119729145</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -2989,19 +2988,19 @@
       </c>
       <c r="E95" s="7">
         <f t="shared" si="12"/>
-        <v>10586888.273314869</v>
+        <v>14115851.03108649</v>
       </c>
       <c r="F95" s="7">
         <f t="shared" si="13"/>
-        <v>10334955.831981253</v>
+        <v>13779941.109308336</v>
       </c>
       <c r="G95" s="8">
         <f t="shared" si="14"/>
-        <v>2117.3776546629738</v>
+        <v>2823.1702062172981</v>
       </c>
       <c r="H95" s="8">
         <f t="shared" si="15"/>
-        <v>105868.8827331487</v>
+        <v>141158.51031086489</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -3016,19 +3015,19 @@
       </c>
       <c r="E96" s="7">
         <f t="shared" si="12"/>
-        <v>2874976.9159741406</v>
+        <v>3833302.5546321874</v>
       </c>
       <c r="F96" s="7">
         <f t="shared" si="13"/>
-        <v>2806562.1056426843</v>
+        <v>3742082.8075235793</v>
       </c>
       <c r="G96" s="8">
         <f t="shared" si="14"/>
-        <v>574.99538319482815</v>
+        <v>766.6605109264375</v>
       </c>
       <c r="H96" s="8">
         <f t="shared" si="15"/>
-        <v>28749.769159741405</v>
+        <v>38333.025546321871</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -3043,19 +3042,19 @@
       </c>
       <c r="E97" s="7">
         <f t="shared" si="12"/>
-        <v>3140904.8938134853</v>
+        <v>4187873.1917513134</v>
       </c>
       <c r="F97" s="7">
         <f t="shared" si="13"/>
-        <v>3066161.8893095404</v>
+        <v>4088215.8524127207</v>
       </c>
       <c r="G97" s="8">
         <f t="shared" si="14"/>
-        <v>628.18097876269701</v>
+        <v>837.57463835026272</v>
       </c>
       <c r="H97" s="8">
         <f t="shared" si="15"/>
-        <v>31409.048938134853</v>
+        <v>41878.731917513134</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -3070,19 +3069,19 @@
       </c>
       <c r="E98" s="7">
         <f t="shared" si="12"/>
-        <v>3672760.8494921504</v>
+        <v>4897014.4659895338</v>
       </c>
       <c r="F98" s="7">
         <f t="shared" si="13"/>
-        <v>3585361.4566432294</v>
+        <v>4780481.9421909722</v>
       </c>
       <c r="G98" s="8">
         <f t="shared" si="14"/>
-        <v>734.55216989843007</v>
+        <v>979.40289319790679</v>
       </c>
       <c r="H98" s="8">
         <f t="shared" si="15"/>
-        <v>36727.6084949215</v>
+        <v>48970.144659895341</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -3097,19 +3096,19 @@
       </c>
       <c r="E99" s="7">
         <f t="shared" si="12"/>
-        <v>5534256.6943675019</v>
+        <v>7379008.9258233355</v>
       </c>
       <c r="F99" s="7">
         <f t="shared" si="13"/>
-        <v>5402559.9423111631</v>
+        <v>7203413.2564148847</v>
       </c>
       <c r="G99" s="8">
         <f t="shared" si="14"/>
-        <v>1106.8513388735005</v>
+        <v>1475.8017851646671</v>
       </c>
       <c r="H99" s="8">
         <f t="shared" si="15"/>
-        <v>55342.566943675018</v>
+        <v>73790.089258233362</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -3124,19 +3123,19 @@
       </c>
       <c r="E100" s="7">
         <f t="shared" si="12"/>
-        <v>6332040.6278855</v>
+        <v>8442720.8371806666</v>
       </c>
       <c r="F100" s="7">
         <f t="shared" si="13"/>
-        <v>6181359.2933116956</v>
+        <v>8241812.3910822617</v>
       </c>
       <c r="G100" s="8">
         <f t="shared" si="14"/>
-        <v>1266.4081255771</v>
+        <v>1688.5441674361334</v>
       </c>
       <c r="H100" s="8">
         <f t="shared" si="15"/>
-        <v>63320.406278855</v>
+        <v>84427.208371806671</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -3151,19 +3150,19 @@
       </c>
       <c r="E101" s="7">
         <f t="shared" si="12"/>
-        <v>8459464.4506001845</v>
+        <v>11279285.934133578</v>
       </c>
       <c r="F101" s="7">
         <f t="shared" si="13"/>
-        <v>8258157.5626464738</v>
+        <v>11010876.750195298</v>
       </c>
       <c r="G101" s="8">
         <f t="shared" si="14"/>
-        <v>1691.892890120037</v>
+        <v>2255.8571868267154</v>
       </c>
       <c r="H101" s="8">
         <f t="shared" si="15"/>
-        <v>84594.644506001845</v>
+        <v>112792.85934133577</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
@@ -3185,19 +3184,19 @@
       </c>
       <c r="E103" s="7">
         <f t="shared" si="12"/>
-        <v>10679944.674965421</v>
+        <v>14239926.233287228</v>
       </c>
       <c r="F103" s="7">
         <f t="shared" si="13"/>
-        <v>10437415.517707488</v>
+        <v>13916554.023609987</v>
       </c>
       <c r="G103" s="8">
         <f t="shared" ref="G103:G111" si="16">E103/$B$5</f>
-        <v>2135.9889349930841</v>
+        <v>2847.9852466574457</v>
       </c>
       <c r="H103" s="8">
         <f t="shared" ref="H103:H111" si="17">E103/$B$6</f>
-        <v>106799.44674965421</v>
+        <v>142399.26233287228</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -3212,19 +3211,19 @@
       </c>
       <c r="E104" s="7">
         <f t="shared" si="12"/>
-        <v>11874965.421853393</v>
+        <v>15833287.22913786</v>
       </c>
       <c r="F104" s="7">
         <f t="shared" si="13"/>
-        <v>11605298.729386326</v>
+        <v>15473731.63918177</v>
       </c>
       <c r="G104" s="8">
         <f t="shared" si="16"/>
-        <v>2374.9930843706788</v>
+        <v>3166.6574458275722</v>
       </c>
       <c r="H104" s="8">
         <f t="shared" si="17"/>
-        <v>118749.65421853393</v>
+        <v>158332.87229137859</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -3239,19 +3238,19 @@
       </c>
       <c r="E105" s="7">
         <f t="shared" si="12"/>
-        <v>13069986.168741349</v>
+        <v>17426648.224988464</v>
       </c>
       <c r="F105" s="7">
         <f t="shared" si="13"/>
-        <v>12773181.941065146</v>
+        <v>17030909.25475353</v>
       </c>
       <c r="G105" s="8">
         <f t="shared" si="16"/>
-        <v>2613.99723374827</v>
+        <v>3485.3296449976929</v>
       </c>
       <c r="H105" s="8">
         <f t="shared" si="17"/>
-        <v>130699.86168741349</v>
+        <v>174266.48224988463</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
@@ -3266,19 +3265,19 @@
       </c>
       <c r="E106" s="7">
         <f t="shared" si="12"/>
-        <v>14663347.164591974</v>
+        <v>19551129.552789297</v>
       </c>
       <c r="F106" s="7">
         <f t="shared" si="13"/>
-        <v>14330359.556636924</v>
+        <v>19107146.0755159</v>
       </c>
       <c r="G106" s="8">
         <f t="shared" si="16"/>
-        <v>2932.6694329183947</v>
+        <v>3910.2259105578596</v>
       </c>
       <c r="H106" s="8">
         <f t="shared" si="17"/>
-        <v>146633.47164591972</v>
+        <v>195511.29552789297</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -3293,19 +3292,19 @@
       </c>
       <c r="E107" s="7">
         <f t="shared" si="12"/>
-        <v>15858367.911479946</v>
+        <v>21144490.548639927</v>
       </c>
       <c r="F107" s="7">
         <f t="shared" si="13"/>
-        <v>15498242.768315762</v>
+        <v>20664323.691087686</v>
       </c>
       <c r="G107" s="8">
         <f t="shared" si="16"/>
-        <v>3171.673582295989</v>
+        <v>4228.8981097279857</v>
       </c>
       <c r="H107" s="8">
         <f t="shared" si="17"/>
-        <v>158583.67911479945</v>
+        <v>211444.90548639928</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
@@ -3320,19 +3319,19 @@
       </c>
       <c r="E108" s="7">
         <f t="shared" si="12"/>
-        <v>8289903.1811894942</v>
+        <v>11053204.241585992</v>
       </c>
       <c r="F108" s="7">
         <f t="shared" si="13"/>
-        <v>8101649.0943498304</v>
+        <v>10802198.792466441</v>
       </c>
       <c r="G108" s="8">
         <f t="shared" si="16"/>
-        <v>1657.9806362378988</v>
+        <v>2210.6408483171986</v>
       </c>
       <c r="H108" s="8">
         <f t="shared" si="17"/>
-        <v>82899.031811894936</v>
+        <v>110532.04241585992</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
@@ -3347,19 +3346,19 @@
       </c>
       <c r="E109" s="7">
         <f t="shared" si="12"/>
-        <v>9484923.9280774482</v>
+        <v>12646565.237436598</v>
       </c>
       <c r="F109" s="7">
         <f t="shared" si="13"/>
-        <v>9269532.3060286511</v>
+        <v>12359376.408038201</v>
       </c>
       <c r="G109" s="8">
         <f t="shared" si="16"/>
-        <v>1896.9847856154897</v>
+        <v>2529.3130474873196</v>
       </c>
       <c r="H109" s="8">
         <f t="shared" si="17"/>
-        <v>94849.239280774476</v>
+        <v>126465.65237436598</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -3374,19 +3373,19 @@
       </c>
       <c r="E110" s="7">
         <f t="shared" si="12"/>
-        <v>10281604.426002767</v>
+        <v>13708805.901337024</v>
       </c>
       <c r="F110" s="7">
         <f t="shared" si="13"/>
-        <v>10048121.113814546</v>
+        <v>13397494.818419397</v>
       </c>
       <c r="G110" s="8">
         <f t="shared" si="16"/>
-        <v>2056.3208852005532</v>
+        <v>2741.7611802674046</v>
       </c>
       <c r="H110" s="8">
         <f t="shared" si="17"/>
-        <v>102816.04426002767</v>
+        <v>137088.05901337025</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -3401,19 +3400,19 @@
       </c>
       <c r="E111" s="7">
         <f t="shared" si="12"/>
-        <v>12671645.919778697</v>
+        <v>16895527.893038265</v>
       </c>
       <c r="F111" s="7">
         <f t="shared" si="13"/>
-        <v>12383887.537172206</v>
+        <v>16511850.049562944</v>
       </c>
       <c r="G111" s="8">
         <f t="shared" si="16"/>
-        <v>2534.3291839557396</v>
+        <v>3379.1055786076531</v>
       </c>
       <c r="H111" s="8">
         <f t="shared" si="17"/>
-        <v>126716.45919778697</v>
+        <v>168955.27893038266</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -3435,19 +3434,19 @@
       </c>
       <c r="E113" s="7">
         <f t="shared" si="12"/>
-        <v>15811418.047882145</v>
+        <v>21081890.730509527</v>
       </c>
       <c r="F113" s="7">
         <f t="shared" si="13"/>
-        <v>15436174.038115792</v>
+        <v>20581565.384154391</v>
       </c>
       <c r="G113" s="8">
         <f t="shared" ref="G113:G122" si="18">E113/$B$5</f>
-        <v>3162.2836095764292</v>
+        <v>4216.3781461019053</v>
       </c>
       <c r="H113" s="8">
         <f t="shared" ref="H113:H122" si="19">E113/$B$6</f>
-        <v>158114.18047882145</v>
+        <v>210818.90730509526</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -3462,19 +3461,19 @@
       </c>
       <c r="E114" s="7">
         <f t="shared" si="12"/>
-        <v>17402578.268876605</v>
+        <v>23203437.69183547</v>
       </c>
       <c r="F114" s="7">
         <f t="shared" si="13"/>
-        <v>16989572.096368205</v>
+        <v>22652762.795157608</v>
       </c>
       <c r="G114" s="8">
         <f t="shared" si="18"/>
-        <v>3480.515653775321</v>
+        <v>4640.687538367094</v>
       </c>
       <c r="H114" s="8">
         <f t="shared" si="19"/>
-        <v>174025.78268876605</v>
+        <v>232034.37691835471</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
@@ -3489,19 +3488,19 @@
       </c>
       <c r="E115" s="7">
         <f t="shared" si="12"/>
-        <v>18463351.749539599</v>
+        <v>24617802.332719468</v>
       </c>
       <c r="F115" s="7">
         <f t="shared" si="13"/>
-        <v>18025170.801869836</v>
+        <v>24033561.069159783</v>
       </c>
       <c r="G115" s="8">
         <f t="shared" si="18"/>
-        <v>3692.6703499079199</v>
+        <v>4923.5604665438932</v>
       </c>
       <c r="H115" s="8">
         <f t="shared" si="19"/>
-        <v>184633.51749539599</v>
+        <v>246178.02332719468</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -3516,19 +3515,19 @@
       </c>
       <c r="E116" s="7">
         <f t="shared" si="12"/>
-        <v>19524125.230202574</v>
+        <v>26032166.973603431</v>
       </c>
       <c r="F116" s="7">
         <f t="shared" si="13"/>
-        <v>19060769.507371444</v>
+        <v>25414359.343161926</v>
       </c>
       <c r="G116" s="8">
         <f t="shared" si="18"/>
-        <v>3904.8250460405147</v>
+        <v>5206.433394720686</v>
       </c>
       <c r="H116" s="8">
         <f t="shared" si="19"/>
-        <v>195241.25230202574</v>
+        <v>260321.66973603432</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -3543,19 +3542,19 @@
       </c>
       <c r="E117" s="7">
         <f t="shared" si="12"/>
-        <v>21115285.451197058</v>
+        <v>28153713.934929408</v>
       </c>
       <c r="F117" s="7">
         <f t="shared" si="13"/>
-        <v>20614167.565623879</v>
+        <v>27485556.754165173</v>
       </c>
       <c r="G117" s="8">
         <f t="shared" si="18"/>
-        <v>4223.057090239412</v>
+        <v>5630.742786985882</v>
       </c>
       <c r="H117" s="8">
         <f t="shared" si="19"/>
-        <v>211152.85451197057</v>
+        <v>281537.13934929407</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
@@ -3570,19 +3569,19 @@
       </c>
       <c r="E118" s="7">
         <f t="shared" si="12"/>
-        <v>11037937.384898718</v>
+        <v>14717249.846531626</v>
       </c>
       <c r="F118" s="7">
         <f t="shared" si="13"/>
-        <v>10775979.863358511</v>
+        <v>14367973.151144683</v>
       </c>
       <c r="G118" s="8">
         <f t="shared" si="18"/>
-        <v>2207.5874769797438</v>
+        <v>2943.4499693063253</v>
       </c>
       <c r="H118" s="8">
         <f t="shared" si="19"/>
-        <v>110379.37384898719</v>
+        <v>147172.49846531625</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
@@ -3597,19 +3596,19 @@
       </c>
       <c r="E119" s="7">
         <f t="shared" si="12"/>
-        <v>12629097.605893178</v>
+        <v>16838796.807857573</v>
       </c>
       <c r="F119" s="7">
         <f t="shared" si="13"/>
-        <v>12329377.921610923</v>
+        <v>16439170.562147899</v>
       </c>
       <c r="G119" s="8">
         <f t="shared" si="18"/>
-        <v>2525.8195211786356</v>
+        <v>3367.7593615715145</v>
       </c>
       <c r="H119" s="8">
         <f t="shared" si="19"/>
-        <v>126290.97605893177</v>
+        <v>168387.96807857574</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
@@ -3624,19 +3623,19 @@
       </c>
       <c r="E120" s="7">
         <f t="shared" si="12"/>
-        <v>13689871.086556172</v>
+        <v>18253161.448741563</v>
       </c>
       <c r="F120" s="7">
         <f t="shared" si="13"/>
-        <v>13364976.627112551</v>
+        <v>17819968.836150069</v>
       </c>
       <c r="G120" s="8">
         <f t="shared" si="18"/>
-        <v>2737.9742173112345</v>
+        <v>3650.6322897483124</v>
       </c>
       <c r="H120" s="8">
         <f t="shared" si="19"/>
-        <v>136898.71086556173</v>
+        <v>182531.61448741562</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
@@ -3651,19 +3650,19 @@
       </c>
       <c r="E121" s="7">
         <f t="shared" si="12"/>
-        <v>14220257.826887662</v>
+        <v>18960343.76918355</v>
       </c>
       <c r="F121" s="7">
         <f t="shared" si="13"/>
-        <v>13882775.979863357</v>
+        <v>18510367.973151144</v>
       </c>
       <c r="G121" s="8">
         <f t="shared" si="18"/>
-        <v>2844.0515653775324</v>
+        <v>3792.0687538367101</v>
       </c>
       <c r="H121" s="8">
         <f t="shared" si="19"/>
-        <v>142202.57826887662</v>
+        <v>189603.43769183551</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
@@ -3678,19 +3677,19 @@
       </c>
       <c r="E122" s="7">
         <f t="shared" si="12"/>
-        <v>16872191.528545119</v>
+        <v>22496255.371393491</v>
       </c>
       <c r="F122" s="7">
         <f t="shared" si="13"/>
-        <v>16471772.743617401</v>
+        <v>21962363.658156537</v>
       </c>
       <c r="G122" s="8">
         <f t="shared" si="18"/>
-        <v>3374.4383057090236</v>
+        <v>4499.2510742786981</v>
       </c>
       <c r="H122" s="8">
         <f t="shared" si="19"/>
-        <v>168721.91528545119</v>
+        <v>224962.5537139349</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
@@ -3713,19 +3712,19 @@
       </c>
       <c r="E124" s="7">
         <f t="shared" si="12"/>
-        <v>21723218.390804589</v>
+        <v>28964291.187739454</v>
       </c>
       <c r="F124" s="7">
         <f t="shared" si="13"/>
-        <v>21254161.04363472</v>
+        <v>28338881.391512956</v>
       </c>
       <c r="G124" s="8">
         <f t="shared" ref="G124:G129" si="20">E124/$B$5</f>
-        <v>4344.6436781609182</v>
+        <v>5792.8582375478909</v>
       </c>
       <c r="H124" s="8">
         <f t="shared" ref="H124:H129" si="21">E124/$B$6</f>
-        <v>217232.18390804587</v>
+        <v>289642.91187739454</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
@@ -3740,19 +3739,19 @@
       </c>
       <c r="E125" s="7">
         <f t="shared" si="12"/>
-        <v>23047356.321839087</v>
+        <v>30729808.429118786</v>
       </c>
       <c r="F125" s="7">
         <f t="shared" si="13"/>
-        <v>22549707.602339189</v>
+        <v>30066276.803118918</v>
       </c>
       <c r="G125" s="8">
         <f t="shared" si="20"/>
-        <v>4609.4712643678176</v>
+        <v>6145.9616858237569</v>
       </c>
       <c r="H125" s="8">
         <f t="shared" si="21"/>
-        <v>230473.56321839086</v>
+        <v>307298.08429118787</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
@@ -3767,19 +3766,19 @@
       </c>
       <c r="E126" s="7">
         <f t="shared" si="12"/>
-        <v>24371494.252873555</v>
+        <v>32495325.670498077</v>
       </c>
       <c r="F126" s="7">
         <f t="shared" si="13"/>
-        <v>23845254.161043629</v>
+        <v>31793672.214724835</v>
       </c>
       <c r="G126" s="8">
         <f t="shared" si="20"/>
-        <v>4874.2988505747107</v>
+        <v>6499.0651340996155</v>
       </c>
       <c r="H126" s="8">
         <f t="shared" si="21"/>
-        <v>243714.94252873556</v>
+        <v>324953.25670498074</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
@@ -3794,19 +3793,19 @@
       </c>
       <c r="E127" s="7">
         <f t="shared" si="12"/>
-        <v>26357701.149425291</v>
+        <v>35143601.532567054</v>
       </c>
       <c r="F127" s="7">
         <f t="shared" si="13"/>
-        <v>25788573.99910032</v>
+        <v>34384765.332133755</v>
       </c>
       <c r="G127" s="8">
         <f t="shared" si="20"/>
-        <v>5271.5402298850577</v>
+        <v>7028.7203065134108</v>
       </c>
       <c r="H127" s="8">
         <f t="shared" si="21"/>
-        <v>263577.01149425289</v>
+        <v>351436.01532567054</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
@@ -3821,19 +3820,19 @@
       </c>
       <c r="E128" s="7">
         <f t="shared" si="12"/>
-        <v>19737011.494252883</v>
+        <v>26316015.325670514</v>
       </c>
       <c r="F128" s="7">
         <f t="shared" si="13"/>
-        <v>19310841.205578059</v>
+        <v>25747788.274104077</v>
       </c>
       <c r="G128" s="8">
         <f t="shared" si="20"/>
-        <v>3947.4022988505767</v>
+        <v>5263.2030651341029</v>
       </c>
       <c r="H128" s="8">
         <f t="shared" si="21"/>
-        <v>197370.11494252883</v>
+        <v>263160.15325670515</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
@@ -3848,19 +3847,19 @@
       </c>
       <c r="E129" s="7">
         <f t="shared" si="12"/>
-        <v>21061149.425287351</v>
+        <v>28081532.567049805</v>
       </c>
       <c r="F129" s="7">
         <f t="shared" si="13"/>
-        <v>20606387.764282499</v>
+        <v>27475183.685709998</v>
       </c>
       <c r="G129" s="8">
         <f t="shared" si="20"/>
-        <v>4212.2298850574698</v>
+        <v>5616.3065134099606</v>
       </c>
       <c r="H129" s="8">
         <f t="shared" si="21"/>
-        <v>210611.4942528735</v>
+        <v>280815.32567049807</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
@@ -3913,19 +3912,19 @@
       </c>
       <c r="E134" s="7">
         <f t="shared" si="12"/>
-        <v>2609048.9381348081</v>
+        <v>3478731.9175130776</v>
       </c>
       <c r="F134" s="7">
         <f t="shared" si="13"/>
-        <v>2546962.3219758403</v>
+        <v>3395949.7626344538</v>
       </c>
       <c r="G134" s="8">
         <f>E134/$B$5</f>
-        <v>521.80978762696157</v>
+        <v>695.74638350261557</v>
       </c>
       <c r="H134" s="8">
         <f>E134/$B$6</f>
-        <v>26090.489381348081</v>
+        <v>34787.319175130775</v>
       </c>
     </row>
     <row r="135" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -3952,19 +3951,19 @@
       </c>
       <c r="E136" s="7">
         <f t="shared" si="12"/>
-        <v>1173185.3906611188</v>
+        <v>1564247.1875481585</v>
       </c>
       <c r="F136" s="7">
         <f t="shared" si="13"/>
-        <v>1145229.7138730932</v>
+        <v>1526972.9518307908</v>
       </c>
       <c r="G136" s="8">
         <f>E136/$B$5</f>
-        <v>234.63707813222376</v>
+        <v>312.84943750963168</v>
       </c>
       <c r="H136" s="8">
         <f>E136/$B$6</f>
-        <v>11731.853906611188</v>
+        <v>15642.471875481584</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
@@ -3979,19 +3978,19 @@
       </c>
       <c r="E137" s="7">
         <f t="shared" si="12"/>
-        <v>1439482.2006472466</v>
+        <v>1919309.6008629953</v>
       </c>
       <c r="F137" s="7">
         <f t="shared" si="13"/>
-        <v>1405180.973012002</v>
+        <v>1873574.6306826693</v>
       </c>
       <c r="G137" s="8">
         <f>E137/$B$5</f>
-        <v>287.89644012944933</v>
+        <v>383.86192017259907</v>
       </c>
       <c r="H137" s="8">
         <f>E137/$B$6</f>
-        <v>14394.822006472466</v>
+        <v>19193.096008629953</v>
       </c>
     </row>
     <row r="138" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4006,19 +4005,19 @@
       </c>
       <c r="E138" s="7">
         <f t="shared" si="12"/>
-        <v>1972075.8206195079</v>
+        <v>2629434.4274926772</v>
       </c>
       <c r="F138" s="7">
         <f t="shared" si="13"/>
-        <v>1925083.4912898254</v>
+        <v>2566777.988386434</v>
       </c>
       <c r="G138" s="8">
         <f>E138/$B$5</f>
-        <v>394.4151641239016</v>
+        <v>525.88688549853543</v>
       </c>
       <c r="H138" s="8">
         <f>E138/$B$6</f>
-        <v>19720.758206195078</v>
+        <v>26294.344274926771</v>
       </c>
     </row>
     <row r="139" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4045,19 +4044,19 @@
       </c>
       <c r="E140" s="7">
         <f t="shared" si="12"/>
-        <v>1173185.3906611188</v>
+        <v>1564247.1875481585</v>
       </c>
       <c r="F140" s="7">
         <f t="shared" si="13"/>
-        <v>1145229.7138730932</v>
+        <v>1526972.9518307908</v>
       </c>
       <c r="G140" s="8">
         <f>E140/$B$5</f>
-        <v>234.63707813222376</v>
+        <v>312.84943750963168</v>
       </c>
       <c r="H140" s="8">
         <f>E140/$B$6</f>
-        <v>11731.853906611188</v>
+        <v>15642.471875481584</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
@@ -4072,19 +4071,19 @@
       </c>
       <c r="E141" s="7">
         <f t="shared" ref="E141:E144" si="22">$B$7/($B$11/D141+90+ROUNDUP(($B$11/D141/90/16-1),0)*0)*($B$11*(B141)-(16*12)-80)</f>
-        <v>1572630.6056403164</v>
+        <v>2096840.8075204217</v>
       </c>
       <c r="F141" s="7">
         <f t="shared" ref="F141:F144" si="23">$B$7/($B$11/D141+90+ROUNDUP(($B$11/D141/90/16-1),0)*36)*($B$11*(B141)-(16*12)-80)</f>
-        <v>1535156.6025814624</v>
+        <v>2046875.4701086164</v>
       </c>
       <c r="G141" s="8">
         <f>E141/$B$5</f>
-        <v>314.52612112806327</v>
+        <v>419.36816150408436</v>
       </c>
       <c r="H141" s="8">
         <f>E141/$B$6</f>
-        <v>15726.306056403164</v>
+        <v>20968.408075204217</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
@@ -4099,19 +4098,19 @@
       </c>
       <c r="E142" s="7">
         <f t="shared" si="22"/>
-        <v>1972075.8206195079</v>
+        <v>2629434.4274926772</v>
       </c>
       <c r="F142" s="7">
         <f t="shared" si="23"/>
-        <v>1925083.4912898254</v>
+        <v>2566777.988386434</v>
       </c>
       <c r="G142" s="8">
         <f>E142/$B$5</f>
-        <v>394.4151641239016</v>
+        <v>525.88688549853543</v>
       </c>
       <c r="H142" s="8">
         <f>E142/$B$6</f>
-        <v>19720.758206195078</v>
+        <v>26294.344274926771</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
@@ -4126,19 +4125,19 @@
       </c>
       <c r="E143" s="7">
         <f t="shared" si="22"/>
-        <v>1173185.3906611188</v>
+        <v>1564247.1875481585</v>
       </c>
       <c r="F143" s="7">
         <f t="shared" si="23"/>
-        <v>1145229.7138730932</v>
+        <v>1526972.9518307908</v>
       </c>
       <c r="G143" s="8">
         <f>E143/$B$5</f>
-        <v>234.63707813222376</v>
+        <v>312.84943750963168</v>
       </c>
       <c r="H143" s="8">
         <f>E143/$B$6</f>
-        <v>11731.853906611188</v>
+        <v>15642.471875481584</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
@@ -4153,19 +4152,19 @@
       </c>
       <c r="E144" s="7">
         <f t="shared" si="22"/>
-        <v>1439482.2006472466</v>
+        <v>1919309.6008629953</v>
       </c>
       <c r="F144" s="7">
         <f t="shared" si="23"/>
-        <v>1405180.973012002</v>
+        <v>1873574.6306826693</v>
       </c>
       <c r="G144" s="8">
         <f>E144/$B$5</f>
-        <v>287.89644012944933</v>
+        <v>383.86192017259907</v>
       </c>
       <c r="H144" s="8">
         <f>E144/$B$6</f>
-        <v>14394.822006472466</v>
+        <v>19193.096008629953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wiggled the sizes of the columns
</commit_message>
<xml_diff>
--- a/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
+++ b/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6680" yWindow="1660" windowWidth="39120" windowHeight="24660" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="3360" windowWidth="39120" windowHeight="24660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -787,15 +787,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="D144" sqref="D144"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="8" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
improved the middle part, made more sections
</commit_message>
<xml_diff>
--- a/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
+++ b/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="3360" windowWidth="39120" windowHeight="24660" tabRatio="500"/>
+    <workbookView xWindow="3800" yWindow="2960" windowWidth="39120" windowHeight="24660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B144" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4120,26 +4120,26 @@
         <v>110</v>
       </c>
       <c r="B143" s="10">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D143" s="4">
         <v>2</v>
       </c>
       <c r="E143" s="7">
         <f t="shared" si="22"/>
-        <v>3124161.2803939674</v>
+        <v>7910864.8815020006</v>
       </c>
       <c r="F143" s="7">
         <f t="shared" si="23"/>
-        <v>3049816.7177453279</v>
+        <v>7722612.8237485727</v>
       </c>
       <c r="G143" s="8">
         <f>E143/$B$5</f>
-        <v>624.83225607879353</v>
+        <v>1582.1729763004</v>
       </c>
       <c r="H143" s="8">
         <f>E143/$B$6</f>
-        <v>31241.612803939675</v>
+        <v>79108.648815020002</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
found typo with 1/5 and 1/2
</commit_message>
<xml_diff>
--- a/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
+++ b/Engineering/Link_Budget/Phase4_DVBS2X_MODCOD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="2960" windowWidth="39120" windowHeight="24660" tabRatio="500"/>
+    <workbookView xWindow="26340" yWindow="3580" windowWidth="16780" windowHeight="24660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B144" sqref="B144"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>